<commit_message>
Added LR changes to the table
</commit_message>
<xml_diff>
--- a/LSTM_all_experiments.xlsx
+++ b/LSTM_all_experiments.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="106">
   <si>
     <t>RNN</t>
   </si>
@@ -246,6 +246,39 @@
   </si>
   <si>
     <t>0.0572</t>
+  </si>
+  <si>
+    <t>LR_changes</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>0.03</t>
+  </si>
+  <si>
+    <t>0.944</t>
+  </si>
+  <si>
+    <t>0.062</t>
+  </si>
+  <si>
+    <t>0.003</t>
+  </si>
+  <si>
+    <t>0.954</t>
+  </si>
+  <si>
+    <t>0.0457</t>
+  </si>
+  <si>
+    <t>0.00003</t>
+  </si>
+  <si>
+    <t>0.960</t>
+  </si>
+  <si>
+    <t>0.0705</t>
   </si>
   <si>
     <t>Boosting</t>
@@ -307,9 +340,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
@@ -335,9 +368,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -363,13 +425,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -378,9 +433,54 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -394,16 +494,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -416,72 +509,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -492,31 +525,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -534,31 +669,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -570,49 +687,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -625,54 +706,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -686,11 +719,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -699,7 +738,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -715,6 +754,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -754,32 +808,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -788,137 +821,137 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -936,7 +969,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1258,10 +1291,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:H58"/>
+  <dimension ref="A3:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -2086,134 +2119,242 @@
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="1" t="s">
+    <row r="47" spans="1:2">
+      <c r="A47" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-    </row>
-    <row r="49" spans="2:8">
+      <c r="B47" s="4"/>
+    </row>
+    <row r="48" spans="2:8">
+      <c r="B48" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" t="s">
+        <v>18</v>
+      </c>
+      <c r="F48" t="s">
+        <v>19</v>
+      </c>
+      <c r="G48" t="s">
+        <v>5</v>
+      </c>
+      <c r="H48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49">
+        <v>1</v>
+      </c>
       <c r="B49" t="s">
-        <v>78</v>
+        <v>79</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>1000</v>
+      </c>
+      <c r="E49">
+        <v>16</v>
+      </c>
+      <c r="F49">
+        <v>32</v>
       </c>
       <c r="G49" t="s">
+        <v>80</v>
+      </c>
+      <c r="H49" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>1000</v>
+      </c>
+      <c r="E50">
+        <v>16</v>
+      </c>
+      <c r="F50">
+        <v>32</v>
+      </c>
+      <c r="G50" t="s">
+        <v>83</v>
+      </c>
+      <c r="H50" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>1000</v>
+      </c>
+      <c r="E51">
+        <v>16</v>
+      </c>
+      <c r="F51">
+        <v>32</v>
+      </c>
+      <c r="G51" t="s">
+        <v>86</v>
+      </c>
+      <c r="H51" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+    </row>
+    <row r="54" spans="2:8">
+      <c r="B54" t="s">
+        <v>89</v>
+      </c>
+      <c r="G54" t="s">
         <v>5</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H54" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8">
-      <c r="B50">
-        <v>4</v>
-      </c>
-      <c r="G50" t="s">
-        <v>79</v>
-      </c>
-      <c r="H50" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8">
-      <c r="B51">
-        <v>6</v>
-      </c>
-      <c r="G51" t="s">
-        <v>81</v>
-      </c>
-      <c r="H51" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8">
-      <c r="B52">
-        <v>8</v>
-      </c>
-      <c r="G52" t="s">
-        <v>83</v>
-      </c>
-      <c r="H52" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8">
-      <c r="B53">
-        <v>10</v>
-      </c>
-      <c r="G53" t="s">
-        <v>85</v>
-      </c>
-      <c r="H53" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8">
-      <c r="B54">
-        <v>12</v>
-      </c>
-      <c r="G54" t="s">
-        <v>87</v>
-      </c>
-      <c r="H54" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="55" spans="2:8">
       <c r="B55">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G55" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H55" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" spans="2:8">
       <c r="B56">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="G56" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="H56" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="2:8">
       <c r="B57">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="G57" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="H57" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="2:8">
       <c r="B58">
+        <v>10</v>
+      </c>
+      <c r="G58" t="s">
+        <v>96</v>
+      </c>
+      <c r="H58" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8">
+      <c r="B59">
+        <v>12</v>
+      </c>
+      <c r="G59" t="s">
+        <v>98</v>
+      </c>
+      <c r="H59" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8">
+      <c r="B60">
+        <v>14</v>
+      </c>
+      <c r="G60" t="s">
+        <v>99</v>
+      </c>
+      <c r="H60" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8">
+      <c r="B61">
+        <v>16</v>
+      </c>
+      <c r="G61" t="s">
+        <v>100</v>
+      </c>
+      <c r="H61" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8">
+      <c r="B62">
+        <v>18</v>
+      </c>
+      <c r="G62" t="s">
+        <v>102</v>
+      </c>
+      <c r="H62" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8">
+      <c r="B63">
         <v>20</v>
       </c>
-      <c r="G58" t="s">
-        <v>93</v>
-      </c>
-      <c r="H58" t="s">
-        <v>94</v>
+      <c r="G63" t="s">
+        <v>104</v>
+      </c>
+      <c r="H63" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A48:H48"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A53:H53"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Trained a network with freq_map
</commit_message>
<xml_diff>
--- a/LSTM_all_experiments.xlsx
+++ b/LSTM_all_experiments.xlsx
@@ -131,7 +131,7 @@
     <t>0.0704</t>
   </si>
   <si>
-    <t>0.939</t>
+    <t>​</t>
   </si>
   <si>
     <t>0.0761</t>
@@ -358,10 +358,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -392,30 +392,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -429,18 +413,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -452,14 +443,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -467,16 +450,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -491,16 +474,32 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -520,15 +519,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -543,7 +543,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -555,7 +567,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -567,25 +687,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -597,61 +705,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -664,66 +724,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -758,65 +758,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -838,6 +779,41 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -852,139 +828,163 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -992,14 +992,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1344,8 +1341,8 @@
   <sheetPr/>
   <dimension ref="A3:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A15" sqref="$A15:$XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1359,29 +1356,29 @@
     <col min="7" max="7" width="14.3833333333333" style="2" customWidth="1"/>
     <col min="8" max="8" width="15.2583333333333" style="1" customWidth="1"/>
     <col min="9" max="9" width="9" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.25" style="3" customWidth="1"/>
-    <col min="11" max="11" width="10.75" style="4" customWidth="1"/>
+    <col min="10" max="10" width="12.25" style="2" customWidth="1"/>
+    <col min="11" max="11" width="10.75" style="3" customWidth="1"/>
     <col min="12" max="12" width="9" style="2" customWidth="1"/>
-    <col min="13" max="13" width="9" style="4" customWidth="1"/>
+    <col min="13" max="13" width="9" style="3" customWidth="1"/>
     <col min="14" max="14" width="9" style="2" customWidth="1"/>
-    <col min="15" max="15" width="9.375" style="4"/>
+    <col min="15" max="15" width="9.375" style="3"/>
     <col min="16" max="16" width="9" style="2" customWidth="1"/>
-    <col min="17" max="17" width="9" style="4" customWidth="1"/>
+    <col min="17" max="17" width="9" style="3" customWidth="1"/>
     <col min="18" max="1025" width="9" style="1" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:8">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="5"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
@@ -1407,7 +1404,7 @@
       <c r="I5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L5" s="2" t="s">
@@ -1484,31 +1481,31 @@
       <c r="I9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <v>0.00154</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="3">
         <f t="shared" ref="K9:O9" si="0">J9*1000*250*200</f>
         <v>77000</v>
       </c>
       <c r="L9" s="2">
         <v>6.64e-5</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9" s="3">
         <f t="shared" si="0"/>
         <v>3320</v>
       </c>
       <c r="N9" s="2">
         <v>0.164</v>
       </c>
-      <c r="O9" s="4">
+      <c r="O9" s="3">
         <f t="shared" si="0"/>
         <v>8200000</v>
       </c>
       <c r="P9" s="2">
         <v>0.835</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="Q9" s="3">
         <f>P9*1000*250*200</f>
         <v>41750000</v>
       </c>
@@ -1532,46 +1529,46 @@
       <c r="I10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="2">
         <v>0.000265</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="3">
         <f>J10*1000*250*200</f>
         <v>13250</v>
       </c>
       <c r="L10" s="2">
         <v>0.00134</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10" s="3">
         <f>L10*1000*250*200</f>
         <v>67000</v>
       </c>
       <c r="N10" s="2">
         <v>0.00334</v>
       </c>
-      <c r="O10" s="4">
+      <c r="O10" s="3">
         <f>N10*1000*250*200</f>
         <v>167000</v>
       </c>
       <c r="P10" s="2">
         <v>0.995</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="Q10" s="3">
         <f>P10*1000*250*200</f>
         <v>49750000</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="5"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
@@ -1603,7 +1600,7 @@
       <c r="I14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L14" s="2" t="s">
@@ -1641,31 +1638,31 @@
       <c r="I15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="2">
         <v>0.00141</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="3">
         <f t="shared" ref="K15:K25" si="1">J15*1000*250*200</f>
         <v>70500</v>
       </c>
       <c r="L15" s="2">
         <v>0.000194</v>
       </c>
-      <c r="M15" s="4">
+      <c r="M15" s="3">
         <f t="shared" ref="M15:M25" si="2">L15*1000*250*200</f>
         <v>9700</v>
       </c>
       <c r="N15" s="2">
         <v>0.143</v>
       </c>
-      <c r="O15" s="4">
+      <c r="O15" s="3">
         <f t="shared" ref="O15:O25" si="3">N15*1000*250*200</f>
         <v>7150000</v>
       </c>
       <c r="P15" s="2">
         <v>0.855</v>
       </c>
-      <c r="Q15" s="4">
+      <c r="Q15" s="3">
         <f t="shared" ref="Q15:Q25" si="4">P15*1000*250*200</f>
         <v>42750000</v>
       </c>
@@ -1695,31 +1692,31 @@
       <c r="I16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="2">
         <v>0.00156</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="3">
         <f t="shared" si="1"/>
         <v>78000</v>
       </c>
       <c r="L16" s="2">
         <v>5e-5</v>
       </c>
-      <c r="M16" s="4">
+      <c r="M16" s="3">
         <f t="shared" si="2"/>
         <v>2500</v>
       </c>
       <c r="N16" s="2">
         <v>0.169</v>
       </c>
-      <c r="O16" s="4">
+      <c r="O16" s="3">
         <f t="shared" si="3"/>
         <v>8450000</v>
       </c>
       <c r="P16" s="2">
         <v>0.828</v>
       </c>
-      <c r="Q16" s="4">
+      <c r="Q16" s="3">
         <f t="shared" si="4"/>
         <v>41400000</v>
       </c>
@@ -1749,31 +1746,31 @@
       <c r="I17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="2">
         <v>0.00154</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="3">
         <f t="shared" si="1"/>
         <v>77000</v>
       </c>
       <c r="L17" s="2">
         <v>5.87e-5</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17" s="3">
         <f t="shared" si="2"/>
         <v>2935</v>
       </c>
       <c r="N17" s="2">
         <v>0.193</v>
       </c>
-      <c r="O17" s="4">
+      <c r="O17" s="3">
         <f t="shared" si="3"/>
         <v>9650000</v>
       </c>
       <c r="P17" s="2">
         <v>0.806</v>
       </c>
-      <c r="Q17" s="4">
+      <c r="Q17" s="3">
         <f t="shared" si="4"/>
         <v>40300000</v>
       </c>
@@ -1803,31 +1800,31 @@
       <c r="I18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="2">
         <v>0.00144</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18" s="3">
         <f t="shared" si="1"/>
         <v>72000</v>
       </c>
       <c r="L18" s="2">
         <v>0.000164</v>
       </c>
-      <c r="M18" s="4">
+      <c r="M18" s="3">
         <f t="shared" si="2"/>
         <v>8200</v>
       </c>
       <c r="N18" s="2">
         <v>0.147</v>
       </c>
-      <c r="O18" s="4">
+      <c r="O18" s="3">
         <f t="shared" si="3"/>
         <v>7350000</v>
       </c>
       <c r="P18" s="2">
         <v>0.851</v>
       </c>
-      <c r="Q18" s="4">
+      <c r="Q18" s="3">
         <f t="shared" si="4"/>
         <v>42550000</v>
       </c>
@@ -1857,31 +1854,31 @@
       <c r="I19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="2">
         <v>0.00148</v>
       </c>
-      <c r="K19" s="4">
+      <c r="K19" s="3">
         <f t="shared" si="1"/>
         <v>74000</v>
       </c>
       <c r="L19" s="2">
         <v>0.0002</v>
       </c>
-      <c r="M19" s="4">
+      <c r="M19" s="3">
         <f t="shared" si="2"/>
         <v>10000</v>
       </c>
       <c r="N19" s="2">
         <v>0.0683</v>
       </c>
-      <c r="O19" s="4">
+      <c r="O19" s="3">
         <f t="shared" si="3"/>
         <v>3415000</v>
       </c>
       <c r="P19" s="2">
         <v>0.93</v>
       </c>
-      <c r="Q19" s="4">
+      <c r="Q19" s="3">
         <f t="shared" si="4"/>
         <v>46500000</v>
       </c>
@@ -1911,31 +1908,31 @@
       <c r="I20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="2">
         <v>0.00159</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="3">
         <f t="shared" si="1"/>
         <v>79500</v>
       </c>
       <c r="L20" s="2">
         <v>2.49e-5</v>
       </c>
-      <c r="M20" s="4">
+      <c r="M20" s="3">
         <f t="shared" si="2"/>
         <v>1245</v>
       </c>
       <c r="N20" s="2">
         <v>0.424</v>
       </c>
-      <c r="O20" s="4">
+      <c r="O20" s="3">
         <f t="shared" si="3"/>
         <v>21200000</v>
       </c>
       <c r="P20" s="2">
         <v>0.574</v>
       </c>
-      <c r="Q20" s="4">
+      <c r="Q20" s="3">
         <f t="shared" si="4"/>
         <v>28700000</v>
       </c>
@@ -1965,31 +1962,31 @@
       <c r="I21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="2">
         <v>0.0016</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="3">
         <f t="shared" si="1"/>
         <v>80000</v>
       </c>
       <c r="L21" s="2">
         <v>8.04e-6</v>
       </c>
-      <c r="M21" s="4">
+      <c r="M21" s="3">
         <f t="shared" si="2"/>
         <v>402</v>
       </c>
       <c r="N21" s="2">
         <v>0.79</v>
       </c>
-      <c r="O21" s="4">
+      <c r="O21" s="3">
         <f t="shared" si="3"/>
         <v>39500000</v>
       </c>
       <c r="P21" s="2">
         <v>0.209</v>
       </c>
-      <c r="Q21" s="4">
+      <c r="Q21" s="3">
         <f t="shared" si="4"/>
         <v>10450000</v>
       </c>
@@ -2019,31 +2016,31 @@
       <c r="I22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="2">
         <v>0.00143</v>
       </c>
-      <c r="K22" s="4">
+      <c r="K22" s="3">
         <f t="shared" si="1"/>
         <v>71500</v>
       </c>
       <c r="L22" s="2">
         <v>0.000178</v>
       </c>
-      <c r="M22" s="4">
+      <c r="M22" s="3">
         <f t="shared" si="2"/>
         <v>8900</v>
       </c>
       <c r="N22" s="2">
         <v>0.174</v>
       </c>
-      <c r="O22" s="4">
+      <c r="O22" s="3">
         <f t="shared" si="3"/>
         <v>8700000</v>
       </c>
       <c r="P22" s="2">
         <v>0.824</v>
       </c>
-      <c r="Q22" s="4">
+      <c r="Q22" s="3">
         <f t="shared" si="4"/>
         <v>41200000</v>
       </c>
@@ -2073,31 +2070,31 @@
       <c r="I23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="2">
         <v>0.000789</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23" s="3">
         <f t="shared" si="1"/>
         <v>39450</v>
       </c>
       <c r="L23" s="2">
         <v>0.000818</v>
       </c>
-      <c r="M23" s="4">
+      <c r="M23" s="3">
         <f t="shared" si="2"/>
         <v>40900</v>
       </c>
       <c r="N23" s="2">
         <v>0.016</v>
       </c>
-      <c r="O23" s="4">
+      <c r="O23" s="3">
         <f t="shared" si="3"/>
         <v>800000</v>
       </c>
       <c r="P23" s="2">
         <v>0.982</v>
       </c>
-      <c r="Q23" s="4">
+      <c r="Q23" s="3">
         <f t="shared" si="4"/>
         <v>49100000</v>
       </c>
@@ -2127,31 +2124,31 @@
       <c r="I24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="2">
         <v>0.00159</v>
       </c>
-      <c r="K24" s="4">
+      <c r="K24" s="3">
         <f t="shared" si="1"/>
         <v>79500</v>
       </c>
       <c r="L24" s="2">
         <v>1.66e-5</v>
       </c>
-      <c r="M24" s="4">
+      <c r="M24" s="3">
         <f t="shared" si="2"/>
         <v>830</v>
       </c>
       <c r="N24" s="2">
         <v>0.558</v>
       </c>
-      <c r="O24" s="4">
+      <c r="O24" s="3">
         <f t="shared" si="3"/>
         <v>27900000</v>
       </c>
       <c r="P24" s="2">
         <v>0.44</v>
       </c>
-      <c r="Q24" s="4">
+      <c r="Q24" s="3">
         <f t="shared" si="4"/>
         <v>22000000</v>
       </c>
@@ -2181,31 +2178,31 @@
       <c r="I25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="2">
         <v>0.00153</v>
       </c>
-      <c r="K25" s="4">
+      <c r="K25" s="3">
         <f t="shared" si="1"/>
         <v>76500</v>
       </c>
       <c r="L25" s="2">
         <v>7.57e-5</v>
       </c>
-      <c r="M25" s="4">
+      <c r="M25" s="3">
         <f t="shared" si="2"/>
         <v>3785</v>
       </c>
       <c r="N25" s="2">
         <v>0.249</v>
       </c>
-      <c r="O25" s="4">
+      <c r="O25" s="3">
         <f t="shared" si="3"/>
         <v>12450000</v>
       </c>
       <c r="P25" s="2">
         <v>0.75</v>
       </c>
-      <c r="Q25" s="4">
+      <c r="Q25" s="3">
         <f t="shared" si="4"/>
         <v>37500000</v>
       </c>
@@ -2219,31 +2216,30 @@
       </c>
     </row>
     <row r="28" spans="2:16">
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G28" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="H28" s="5" t="s">
         <v>26</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J28" s="3" t="s">
+      <c r="J28" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K28" s="4"/>
       <c r="L28" s="2" t="s">
         <v>9</v>
       </c>
@@ -2279,31 +2275,31 @@
       <c r="I29" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="2">
         <v>4.94e-5</v>
       </c>
-      <c r="K29" s="4">
+      <c r="K29" s="3">
         <f t="shared" ref="K28:K36" si="5">J29*1000*250*200</f>
         <v>2470</v>
       </c>
       <c r="L29" s="2">
         <v>1.6e-5</v>
       </c>
-      <c r="M29" s="4">
+      <c r="M29" s="3">
         <f t="shared" ref="M29:M36" si="6">L29*1000*250*200</f>
         <v>800</v>
       </c>
       <c r="N29" s="2">
         <v>0.0559</v>
       </c>
-      <c r="O29" s="4">
+      <c r="O29" s="3">
         <f t="shared" ref="O29:O36" si="7">N29*1000*250*200</f>
         <v>2795000</v>
       </c>
       <c r="P29" s="2">
         <v>0.944</v>
       </c>
-      <c r="Q29" s="4">
+      <c r="Q29" s="3">
         <f t="shared" ref="Q29:Q36" si="8">P29*1000*250*200</f>
         <v>47200000</v>
       </c>
@@ -2333,31 +2329,31 @@
       <c r="I30" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J30" s="2">
         <v>3.94e-5</v>
       </c>
-      <c r="K30" s="4">
+      <c r="K30" s="3">
         <f t="shared" si="5"/>
         <v>1970</v>
       </c>
       <c r="L30" s="2">
         <v>2.59e-5</v>
       </c>
-      <c r="M30" s="4">
+      <c r="M30" s="3">
         <f t="shared" si="6"/>
         <v>1295</v>
       </c>
       <c r="N30" s="2">
         <v>0.0418</v>
       </c>
-      <c r="O30" s="4">
+      <c r="O30" s="3">
         <f t="shared" si="7"/>
         <v>2090000</v>
       </c>
       <c r="P30" s="2">
         <v>0.958</v>
       </c>
-      <c r="Q30" s="4">
+      <c r="Q30" s="3">
         <f t="shared" si="8"/>
         <v>47900000</v>
       </c>
@@ -2387,31 +2383,31 @@
       <c r="I31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="2">
         <v>5.77e-5</v>
       </c>
-      <c r="K31" s="4">
+      <c r="K31" s="3">
         <f t="shared" si="5"/>
         <v>2885</v>
       </c>
       <c r="L31" s="2">
         <v>7.53e-6</v>
       </c>
-      <c r="M31" s="4">
+      <c r="M31" s="3">
         <f t="shared" si="6"/>
         <v>376.5</v>
       </c>
       <c r="N31" s="2">
         <v>0.123</v>
       </c>
-      <c r="O31" s="4">
+      <c r="O31" s="3">
         <f t="shared" si="7"/>
         <v>6150000</v>
       </c>
       <c r="P31" s="2">
         <v>0.877</v>
       </c>
-      <c r="Q31" s="4">
+      <c r="Q31" s="3">
         <f t="shared" si="8"/>
         <v>43850000</v>
       </c>
@@ -2441,31 +2437,31 @@
       <c r="I32" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32" s="2">
         <v>6.2e-5</v>
       </c>
-      <c r="K32" s="4">
+      <c r="K32" s="3">
         <f t="shared" si="5"/>
         <v>3100</v>
       </c>
       <c r="L32" s="2">
         <v>3.34e-6</v>
       </c>
-      <c r="M32" s="4">
+      <c r="M32" s="3">
         <f t="shared" si="6"/>
         <v>167</v>
       </c>
       <c r="N32" s="2">
         <v>0.289</v>
       </c>
-      <c r="O32" s="4">
+      <c r="O32" s="3">
         <f t="shared" si="7"/>
         <v>14450000</v>
       </c>
       <c r="P32" s="2">
         <v>0.71</v>
       </c>
-      <c r="Q32" s="4">
+      <c r="Q32" s="3">
         <f t="shared" si="8"/>
         <v>35500000</v>
       </c>
@@ -2495,31 +2491,31 @@
       <c r="I33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J33" s="3">
+      <c r="J33" s="2">
         <v>6.2e-5</v>
       </c>
-      <c r="K33" s="4">
+      <c r="K33" s="3">
         <f t="shared" si="5"/>
         <v>3100</v>
       </c>
       <c r="L33" s="2">
         <v>3.34e-6</v>
       </c>
-      <c r="M33" s="4">
+      <c r="M33" s="3">
         <f t="shared" si="6"/>
         <v>167</v>
       </c>
       <c r="N33" s="2">
         <v>0.194</v>
       </c>
-      <c r="O33" s="4">
+      <c r="O33" s="3">
         <f t="shared" si="7"/>
         <v>9700000</v>
       </c>
       <c r="P33" s="2">
         <v>0.806</v>
       </c>
-      <c r="Q33" s="4">
+      <c r="Q33" s="3">
         <f t="shared" si="8"/>
         <v>40300000</v>
       </c>
@@ -2549,31 +2545,31 @@
       <c r="I34" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="2">
         <v>6.28e-5</v>
       </c>
-      <c r="K34" s="4">
+      <c r="K34" s="3">
         <f t="shared" si="5"/>
         <v>3140</v>
       </c>
       <c r="L34" s="2">
         <v>2.49e-6</v>
       </c>
-      <c r="M34" s="4">
+      <c r="M34" s="3">
         <f t="shared" si="6"/>
         <v>124.5</v>
       </c>
       <c r="N34" s="2">
         <v>0.324</v>
       </c>
-      <c r="O34" s="4">
+      <c r="O34" s="3">
         <f t="shared" si="7"/>
         <v>16200000</v>
       </c>
       <c r="P34" s="2">
         <v>0.675</v>
       </c>
-      <c r="Q34" s="4">
+      <c r="Q34" s="3">
         <f t="shared" si="8"/>
         <v>33750000</v>
       </c>
@@ -2603,31 +2599,31 @@
       <c r="I35" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35" s="2">
         <v>5.28e-5</v>
       </c>
-      <c r="K35" s="4">
+      <c r="K35" s="3">
         <f t="shared" si="5"/>
         <v>2640</v>
       </c>
       <c r="L35" s="2">
         <v>1.26e-5</v>
       </c>
-      <c r="M35" s="4">
+      <c r="M35" s="3">
         <f t="shared" si="6"/>
         <v>630</v>
       </c>
       <c r="N35" s="2">
         <v>0.0874</v>
       </c>
-      <c r="O35" s="4">
+      <c r="O35" s="3">
         <f t="shared" si="7"/>
         <v>4370000</v>
       </c>
       <c r="P35" s="2">
         <v>0.913</v>
       </c>
-      <c r="Q35" s="4">
+      <c r="Q35" s="3">
         <f t="shared" si="8"/>
         <v>45650000</v>
       </c>
@@ -2657,40 +2653,40 @@
       <c r="I36" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J36" s="2">
         <v>5.27e-5</v>
       </c>
-      <c r="K36" s="4">
+      <c r="K36" s="3">
         <f t="shared" si="5"/>
         <v>2635</v>
       </c>
       <c r="L36" s="2">
         <v>1.26e-5</v>
       </c>
-      <c r="M36" s="4">
+      <c r="M36" s="3">
         <f t="shared" si="6"/>
         <v>630</v>
       </c>
       <c r="N36" s="2">
         <v>0.131</v>
       </c>
-      <c r="O36" s="4">
+      <c r="O36" s="3">
         <f t="shared" si="7"/>
         <v>6550000</v>
       </c>
       <c r="P36" s="2">
         <v>0.868</v>
       </c>
-      <c r="Q36" s="4">
+      <c r="Q36" s="3">
         <f t="shared" si="8"/>
         <v>43400000</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B38" s="7"/>
+      <c r="B38" s="6"/>
       <c r="C38" s="1" t="s">
         <v>1</v>
       </c>
@@ -2723,7 +2719,7 @@
       <c r="I39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J39" s="3" t="s">
+      <c r="J39" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L39" s="2" t="s">
@@ -2764,31 +2760,31 @@
       <c r="I40" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40" s="2">
         <v>0.00128</v>
       </c>
-      <c r="K40" s="4">
+      <c r="K40" s="3">
         <f t="shared" ref="K40:K45" si="9">J40*1000*250*200</f>
         <v>64000</v>
       </c>
       <c r="L40" s="2">
         <v>0.000273</v>
       </c>
-      <c r="M40" s="4">
+      <c r="M40" s="3">
         <f t="shared" ref="M40:M45" si="10">L40*1000*250*200</f>
         <v>13650</v>
       </c>
       <c r="N40" s="2">
         <v>0.0565</v>
       </c>
-      <c r="O40" s="4">
+      <c r="O40" s="3">
         <f t="shared" ref="O40:O45" si="11">N40*1000*250*200</f>
         <v>2825000</v>
       </c>
       <c r="P40" s="2">
         <v>0.942</v>
       </c>
-      <c r="Q40" s="4">
+      <c r="Q40" s="3">
         <f t="shared" ref="Q40:Q45" si="12">P40*1000*250*200</f>
         <v>47100000</v>
       </c>
@@ -2821,31 +2817,31 @@
       <c r="I41" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J41" s="3">
+      <c r="J41" s="2">
         <v>0.00127</v>
       </c>
-      <c r="K41" s="4">
+      <c r="K41" s="3">
         <f t="shared" si="9"/>
         <v>63500</v>
       </c>
       <c r="L41" s="2">
         <v>0.000335</v>
       </c>
-      <c r="M41" s="4">
+      <c r="M41" s="3">
         <f t="shared" si="10"/>
         <v>16750</v>
       </c>
       <c r="N41" s="2">
         <v>0.0436</v>
       </c>
-      <c r="O41" s="4">
+      <c r="O41" s="3">
         <f t="shared" si="11"/>
         <v>2180000</v>
       </c>
       <c r="P41" s="2">
         <v>0.955</v>
       </c>
-      <c r="Q41" s="4">
+      <c r="Q41" s="3">
         <f t="shared" si="12"/>
         <v>47750000</v>
       </c>
@@ -2878,31 +2874,31 @@
       <c r="I42" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J42" s="2">
         <v>0.0016</v>
       </c>
-      <c r="K42" s="4">
+      <c r="K42" s="3">
         <f t="shared" si="9"/>
         <v>80000</v>
       </c>
       <c r="L42" s="2">
         <v>7.08e-6</v>
       </c>
-      <c r="M42" s="4">
+      <c r="M42" s="3">
         <f t="shared" si="10"/>
         <v>354</v>
       </c>
       <c r="N42" s="2">
         <v>0.93</v>
       </c>
-      <c r="O42" s="4">
+      <c r="O42" s="3">
         <f t="shared" si="11"/>
         <v>46500000</v>
       </c>
       <c r="P42" s="2">
         <v>0.0687</v>
       </c>
-      <c r="Q42" s="4">
+      <c r="Q42" s="3">
         <f t="shared" si="12"/>
         <v>3435000</v>
       </c>
@@ -2935,31 +2931,31 @@
       <c r="I43" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J43" s="3">
+      <c r="J43" s="2">
         <v>0.00108</v>
       </c>
-      <c r="K43" s="4">
+      <c r="K43" s="3">
         <f t="shared" si="9"/>
         <v>54000</v>
       </c>
       <c r="L43" s="2">
         <v>0.000527</v>
       </c>
-      <c r="M43" s="4">
+      <c r="M43" s="3">
         <f t="shared" si="10"/>
         <v>26350</v>
       </c>
       <c r="N43" s="2">
         <v>0.0277</v>
       </c>
-      <c r="O43" s="4">
+      <c r="O43" s="3">
         <f t="shared" si="11"/>
         <v>1385000</v>
       </c>
       <c r="P43" s="2">
         <v>0.971</v>
       </c>
-      <c r="Q43" s="4">
+      <c r="Q43" s="3">
         <f t="shared" si="12"/>
         <v>48550000</v>
       </c>
@@ -2992,31 +2988,31 @@
       <c r="I44" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J44" s="3">
+      <c r="J44" s="2">
         <v>0.00116</v>
       </c>
-      <c r="K44" s="4">
+      <c r="K44" s="3">
         <f t="shared" si="9"/>
         <v>58000</v>
       </c>
       <c r="L44" s="2">
         <v>0.000444</v>
       </c>
-      <c r="M44" s="4">
+      <c r="M44" s="3">
         <f t="shared" si="10"/>
         <v>22200</v>
       </c>
       <c r="N44" s="2">
         <v>0.0308</v>
       </c>
-      <c r="O44" s="4">
+      <c r="O44" s="3">
         <f t="shared" si="11"/>
         <v>1540000</v>
       </c>
       <c r="P44" s="2">
         <v>0.968</v>
       </c>
-      <c r="Q44" s="4">
+      <c r="Q44" s="3">
         <f t="shared" si="12"/>
         <v>48400000</v>
       </c>
@@ -3049,40 +3045,40 @@
       <c r="I45" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J45" s="3">
+      <c r="J45" s="2">
         <v>0.00153</v>
       </c>
-      <c r="K45" s="4">
+      <c r="K45" s="3">
         <f t="shared" si="9"/>
         <v>76500</v>
       </c>
       <c r="L45" s="2">
         <v>8.45e-5</v>
       </c>
-      <c r="M45" s="4">
+      <c r="M45" s="3">
         <f t="shared" si="10"/>
         <v>4225</v>
       </c>
       <c r="N45" s="2">
         <v>0.218</v>
       </c>
-      <c r="O45" s="4">
+      <c r="O45" s="3">
         <f t="shared" si="11"/>
         <v>10900000</v>
       </c>
       <c r="P45" s="2">
         <v>0.78</v>
       </c>
-      <c r="Q45" s="4">
+      <c r="Q45" s="3">
         <f t="shared" si="12"/>
         <v>39000000</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B47" s="7"/>
+      <c r="B47" s="6"/>
     </row>
     <row r="48" spans="2:16">
       <c r="B48" s="1" t="s">
@@ -3109,7 +3105,7 @@
       <c r="I48" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J48" s="3" t="s">
+      <c r="J48" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L48" s="2" t="s">
@@ -3150,31 +3146,31 @@
       <c r="I49" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J49" s="3">
+      <c r="J49" s="2">
         <v>0.00142</v>
       </c>
-      <c r="K49" s="4">
+      <c r="K49" s="3">
         <f t="shared" ref="K49:K51" si="13">J49*1000*250*200</f>
         <v>71000</v>
       </c>
       <c r="L49" s="2">
         <v>0.000217</v>
       </c>
-      <c r="M49" s="4">
+      <c r="M49" s="3">
         <f t="shared" ref="M49:M51" si="14">L49*1000*250*200</f>
         <v>10850</v>
       </c>
       <c r="N49" s="2">
         <v>0.064</v>
       </c>
-      <c r="O49" s="4">
+      <c r="O49" s="3">
         <f t="shared" ref="O49:O51" si="15">N49*1000*250*200</f>
         <v>3200000</v>
       </c>
       <c r="P49" s="2">
         <v>0.934</v>
       </c>
-      <c r="Q49" s="4">
+      <c r="Q49" s="3">
         <f t="shared" ref="Q49:Q51" si="16">P49*1000*250*200</f>
         <v>46700000</v>
       </c>
@@ -3207,31 +3203,31 @@
       <c r="I50" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J50" s="3">
+      <c r="J50" s="2">
         <v>0.00146</v>
       </c>
-      <c r="K50" s="4">
+      <c r="K50" s="3">
         <f t="shared" si="13"/>
         <v>73000</v>
       </c>
       <c r="L50" s="2">
         <v>0.000142</v>
       </c>
-      <c r="M50" s="4">
+      <c r="M50" s="3">
         <f t="shared" si="14"/>
         <v>7100</v>
       </c>
       <c r="N50" s="2">
         <v>0.1</v>
       </c>
-      <c r="O50" s="4">
+      <c r="O50" s="3">
         <f t="shared" si="15"/>
         <v>5000000</v>
       </c>
       <c r="P50" s="2">
         <v>0.898</v>
       </c>
-      <c r="Q50" s="4">
+      <c r="Q50" s="3">
         <f t="shared" si="16"/>
         <v>44900000</v>
       </c>
@@ -3264,46 +3260,46 @@
       <c r="I51" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J51" s="3">
+      <c r="J51" s="2">
         <v>0.00136</v>
       </c>
-      <c r="K51" s="4">
+      <c r="K51" s="3">
         <f t="shared" si="13"/>
         <v>68000</v>
       </c>
       <c r="L51" s="2">
         <v>0.000248</v>
       </c>
-      <c r="M51" s="4">
+      <c r="M51" s="3">
         <f t="shared" si="14"/>
         <v>12400</v>
       </c>
       <c r="N51" s="2">
         <v>0.0552</v>
       </c>
-      <c r="O51" s="4">
+      <c r="O51" s="3">
         <f t="shared" si="15"/>
         <v>2760000</v>
       </c>
       <c r="P51" s="2">
         <v>0.943</v>
       </c>
-      <c r="Q51" s="4">
+      <c r="Q51" s="3">
         <f t="shared" si="16"/>
         <v>47150000</v>
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="8"/>
-      <c r="H53" s="5"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="4"/>
     </row>
     <row r="54" spans="2:8">
       <c r="B54" s="1" t="s">

</xml_diff>

<commit_message>
Compared proportion of positive class with and without earthquakes being circled
- Some more computations for R=25
</commit_message>
<xml_diff>
--- a/LSTM_all_experiments.xlsx
+++ b/LSTM_all_experiments.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="117">
   <si>
     <t>RNN</t>
   </si>
@@ -351,6 +351,21 @@
   </si>
   <si>
     <t>0.0695</t>
+  </si>
+  <si>
+    <t>positive_class proportion</t>
+  </si>
+  <si>
+    <t>with</t>
+  </si>
+  <si>
+    <t>0.051</t>
+  </si>
+  <si>
+    <t>without</t>
+  </si>
+  <si>
+    <t>0.0016</t>
   </si>
 </sst>
 </file>
@@ -359,9 +374,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -378,38 +393,16 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -420,77 +413,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -519,8 +444,45 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -529,6 +491,59 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -543,7 +558,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -555,25 +606,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -585,25 +666,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -615,13 +690,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -633,7 +714,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -645,85 +738,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -758,8 +773,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -779,26 +809,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -810,6 +831,24 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -828,167 +867,143 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1339,10 +1354,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:Q63"/>
+  <dimension ref="A3:Q69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A15" sqref="$A15:$XFD15"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H74" sqref="G65:H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3411,6 +3426,27 @@
         <v>111</v>
       </c>
     </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A3:H3"/>

</xml_diff>

<commit_message>
Experiments with number of convolutions in hid2res layers
- Some experiments with new metric
- Added all results to the table
</commit_message>
<xml_diff>
--- a/LSTM_all_experiments.xlsx
+++ b/LSTM_all_experiments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13065" tabRatio="500"/>
+    <workbookView windowWidth="14295" windowHeight="12645" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="130">
   <si>
     <t>RNN</t>
   </si>
@@ -299,6 +299,39 @@
     <t>0.0705</t>
   </si>
   <si>
+    <t>More layers</t>
+  </si>
+  <si>
+    <t>N_LAYERS</t>
+  </si>
+  <si>
+    <t>0.965</t>
+  </si>
+  <si>
+    <t>0.0660</t>
+  </si>
+  <si>
+    <t>0.0654</t>
+  </si>
+  <si>
+    <t>0.0599</t>
+  </si>
+  <si>
+    <t>0.0548</t>
+  </si>
+  <si>
+    <t>New testing data</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>0.948</t>
+  </si>
+  <si>
+    <t>0.699</t>
+  </si>
+  <si>
     <t>Boosting</t>
   </si>
   <si>
@@ -354,6 +387,12 @@
   </si>
   <si>
     <t>positive_class proportion</t>
+  </si>
+  <si>
+    <t>th=3.5</t>
+  </si>
+  <si>
+    <t>th=5</t>
   </si>
   <si>
     <t>with</t>
@@ -373,10 +412,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -398,16 +437,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -421,10 +452,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -433,28 +487,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -470,21 +502,6 @@
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -512,7 +529,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -526,24 +543,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -558,19 +597,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -588,7 +621,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -600,145 +765,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -774,6 +813,15 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -790,21 +838,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -835,24 +868,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -867,147 +882,171 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1028,6 +1067,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1354,10 +1396,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:Q69"/>
+  <dimension ref="A3:Q83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H74" sqref="G65:H74"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="Q63" sqref="Q62:Q63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1392,7 +1434,7 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="7"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:2">
@@ -1582,7 +1624,7 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="7"/>
+      <c r="G12" s="8"/>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:2">
@@ -2243,7 +2285,7 @@
       <c r="F28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="G28" s="9" t="s">
         <v>5</v>
       </c>
       <c r="H28" s="5" t="s">
@@ -3304,32 +3346,72 @@
         <v>47150000</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="4" t="s">
+    <row r="53" spans="1:6">
+      <c r="A53" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="4"/>
-    </row>
-    <row r="54" spans="2:8">
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+    </row>
+    <row r="54" spans="2:16">
       <c r="B54" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="C54" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="G54" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="55" spans="2:8">
+      <c r="I54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N54" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P54" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17">
+      <c r="A55" s="1">
+        <v>1</v>
+      </c>
       <c r="B55" s="1">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1</v>
+      </c>
+      <c r="D55" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E55" s="1">
+        <v>16</v>
+      </c>
+      <c r="F55" s="1">
+        <v>32</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>96</v>
@@ -3337,123 +3419,537 @@
       <c r="H55" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="56" spans="2:8">
+      <c r="I55" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J55" s="2">
+        <v>0.00153</v>
+      </c>
+      <c r="K55" s="3">
+        <f t="shared" ref="K55:K58" si="17">J55*1000*250*200</f>
+        <v>76500</v>
+      </c>
+      <c r="L55" s="2">
+        <v>7.53e-5</v>
+      </c>
+      <c r="M55" s="3">
+        <f t="shared" ref="M55:M58" si="18">L55*1000*250*200</f>
+        <v>3765</v>
+      </c>
+      <c r="N55" s="2">
+        <v>0.135</v>
+      </c>
+      <c r="O55" s="3">
+        <f t="shared" ref="O55:O58" si="19">N55*1000*250*200</f>
+        <v>6750000</v>
+      </c>
+      <c r="P55" s="2">
+        <v>0.863</v>
+      </c>
+      <c r="Q55" s="3">
+        <f t="shared" ref="Q55:Q58" si="20">P55*1000*250*200</f>
+        <v>43150000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17">
+      <c r="A56" s="1">
+        <v>2</v>
+      </c>
       <c r="B56" s="1">
+        <v>3</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1</v>
+      </c>
+      <c r="D56" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E56" s="1">
+        <v>16</v>
+      </c>
+      <c r="F56" s="1">
+        <v>32</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J56" s="2">
+        <v>0.00146</v>
+      </c>
+      <c r="K56" s="3">
+        <f t="shared" si="17"/>
+        <v>73000</v>
+      </c>
+      <c r="L56" s="2">
+        <v>0.000108</v>
+      </c>
+      <c r="M56" s="3">
+        <f t="shared" si="18"/>
+        <v>5400</v>
+      </c>
+      <c r="N56" s="2">
+        <v>0.0926</v>
+      </c>
+      <c r="O56" s="3">
+        <f t="shared" si="19"/>
+        <v>4630000</v>
+      </c>
+      <c r="P56" s="2">
+        <v>0.906</v>
+      </c>
+      <c r="Q56" s="3">
+        <f t="shared" si="20"/>
+        <v>45300000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17">
+      <c r="A57" s="1">
+        <v>3</v>
+      </c>
+      <c r="B57" s="1">
+        <v>4</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1</v>
+      </c>
+      <c r="D57" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E57" s="1">
+        <v>16</v>
+      </c>
+      <c r="F57" s="1">
+        <v>32</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J57" s="2">
+        <v>0.00158</v>
+      </c>
+      <c r="K57" s="3">
+        <f t="shared" si="17"/>
+        <v>79000</v>
+      </c>
+      <c r="L57" s="2">
+        <v>2.9e-5</v>
+      </c>
+      <c r="M57" s="3">
+        <f t="shared" si="18"/>
+        <v>1450</v>
+      </c>
+      <c r="N57" s="2">
+        <v>0.273</v>
+      </c>
+      <c r="O57" s="3">
+        <f t="shared" si="19"/>
+        <v>13650000</v>
+      </c>
+      <c r="P57" s="2">
+        <v>0.725</v>
+      </c>
+      <c r="Q57" s="3">
+        <f t="shared" si="20"/>
+        <v>36250000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17">
+      <c r="A58" s="1">
+        <v>4</v>
+      </c>
+      <c r="B58" s="1">
+        <v>5</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1</v>
+      </c>
+      <c r="D58" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E58" s="1">
+        <v>16</v>
+      </c>
+      <c r="F58" s="1">
+        <v>32</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J58" s="2">
+        <v>0.00144</v>
+      </c>
+      <c r="K58" s="3">
+        <f t="shared" si="17"/>
+        <v>72000</v>
+      </c>
+      <c r="L58" s="2">
+        <v>0.000163</v>
+      </c>
+      <c r="M58" s="3">
+        <f t="shared" si="18"/>
+        <v>8150</v>
+      </c>
+      <c r="N58" s="2">
+        <v>0.102</v>
+      </c>
+      <c r="O58" s="3">
+        <f t="shared" si="19"/>
+        <v>5100000</v>
+      </c>
+      <c r="P58" s="2">
+        <v>0.897</v>
+      </c>
+      <c r="Q58" s="3">
+        <f t="shared" si="20"/>
+        <v>44850000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+    </row>
+    <row r="61" spans="2:16">
+      <c r="B61" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H61" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G56" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8">
-      <c r="B57" s="1">
+      <c r="I61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J61" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G57" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8">
-      <c r="B58" s="1">
+      <c r="L61" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N61" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G58" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H58" s="1" t="s">
+      <c r="P61" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17">
+      <c r="A62" s="1">
+        <v>1</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="1">
+        <v>1</v>
+      </c>
+      <c r="D62" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E62" s="1">
+        <v>16</v>
+      </c>
+      <c r="F62" s="1">
+        <v>32</v>
+      </c>
+      <c r="G62" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="59" spans="2:8">
-      <c r="B59" s="1">
+      <c r="H62" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J62" s="2">
+        <v>0.0389</v>
+      </c>
+      <c r="K62" s="3">
+        <f t="shared" ref="K62:O62" si="21">J62*1000*250*200</f>
+        <v>1945000</v>
+      </c>
+      <c r="L62" s="2">
+        <v>0.0119</v>
+      </c>
+      <c r="M62" s="3">
+        <f t="shared" si="21"/>
+        <v>595000</v>
+      </c>
+      <c r="N62" s="2">
+        <v>0.0368</v>
+      </c>
+      <c r="O62" s="3">
+        <f t="shared" si="21"/>
+        <v>1840000</v>
+      </c>
+      <c r="P62" s="2">
+        <v>0.912</v>
+      </c>
+      <c r="Q62" s="3">
+        <f>P62*1000*250*200</f>
+        <v>45600000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17">
+      <c r="A63" s="1">
+        <v>2</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" s="1">
+        <v>1</v>
+      </c>
+      <c r="D63" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E63" s="1">
+        <v>16</v>
+      </c>
+      <c r="F63" s="1">
+        <v>32</v>
+      </c>
+      <c r="G63" s="2">
+        <v>0.931</v>
+      </c>
+      <c r="H63" s="1">
+        <v>0.0806</v>
+      </c>
+      <c r="I63" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J63" s="2">
+        <v>0.00453</v>
+      </c>
+      <c r="K63" s="3">
+        <f t="shared" ref="K63:O63" si="22">J63*1000*250*200</f>
+        <v>226500</v>
+      </c>
+      <c r="L63" s="2">
+        <v>0.000321</v>
+      </c>
+      <c r="M63" s="3">
+        <f t="shared" si="22"/>
+        <v>16050</v>
+      </c>
+      <c r="N63" s="2">
+        <v>0.187</v>
+      </c>
+      <c r="O63" s="3">
+        <f t="shared" si="22"/>
+        <v>9350000</v>
+      </c>
+      <c r="P63" s="2">
+        <v>0.808</v>
+      </c>
+      <c r="Q63" s="3">
+        <f>P63*1000*250*200</f>
+        <v>40400000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="8"/>
+      <c r="H66" s="4"/>
+    </row>
+    <row r="67" spans="2:8">
+      <c r="B67" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8">
+      <c r="B68" s="1">
+        <v>4</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8">
+      <c r="B69" s="1">
+        <v>6</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8">
+      <c r="B70" s="1">
+        <v>8</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8">
+      <c r="B71" s="1">
+        <v>10</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8">
+      <c r="B72" s="1">
         <v>12</v>
       </c>
-      <c r="G59" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8">
-      <c r="B60" s="1">
+      <c r="G72" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8">
+      <c r="B73" s="1">
         <v>14</v>
       </c>
-      <c r="G60" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8">
-      <c r="B61" s="1">
+      <c r="G73" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8">
+      <c r="B74" s="1">
         <v>16</v>
       </c>
-      <c r="G61" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8">
-      <c r="B62" s="1">
+      <c r="G74" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8">
+      <c r="B75" s="1">
         <v>18</v>
       </c>
-      <c r="G62" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8">
-      <c r="B63" s="1">
+      <c r="G75" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8">
+      <c r="B76" s="1">
         <v>20</v>
       </c>
-      <c r="G63" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>116</v>
+      <c r="G76" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3">
+      <c r="B81" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C82" s="1">
+        <v>0.0049</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C83" s="1">
+        <v>0.0001</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A53:H53"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A60:F60"/>
+    <mergeCell ref="A66:H66"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Added results to the table
</commit_message>
<xml_diff>
--- a/LSTM_all_experiments.xlsx
+++ b/LSTM_all_experiments.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="130">
   <si>
     <t>RNN</t>
   </si>
@@ -412,10 +412,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -432,15 +432,31 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -452,11 +468,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -468,17 +484,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -505,19 +513,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -535,17 +534,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -559,30 +581,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -597,7 +597,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -609,109 +747,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -723,7 +759,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -735,49 +777,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -813,15 +813,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -838,6 +829,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -886,23 +892,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -911,138 +911,138 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1396,10 +1396,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:Q83"/>
+  <dimension ref="A3:Q95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="Q63" sqref="Q62:Q63"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3723,7 +3723,7 @@
         <v>0.912</v>
       </c>
       <c r="Q62" s="3">
-        <f>P62*1000*250*200</f>
+        <f t="shared" ref="Q62:Q71" si="22">P62*1000*250*200</f>
         <v>45600000</v>
       </c>
     </row>
@@ -3759,185 +3759,565 @@
         <v>0.00453</v>
       </c>
       <c r="K63" s="3">
-        <f t="shared" ref="K63:O63" si="22">J63*1000*250*200</f>
+        <f t="shared" ref="K63:O63" si="23">J63*1000*250*200</f>
         <v>226500</v>
       </c>
       <c r="L63" s="2">
         <v>0.000321</v>
       </c>
       <c r="M63" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>16050</v>
       </c>
       <c r="N63" s="2">
         <v>0.187</v>
       </c>
       <c r="O63" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>9350000</v>
       </c>
       <c r="P63" s="2">
         <v>0.808</v>
       </c>
       <c r="Q63" s="3">
-        <f>P63*1000*250*200</f>
+        <f t="shared" si="22"/>
         <v>40400000</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
-      <c r="A66" s="4" t="s">
+    <row r="65" spans="2:16">
+      <c r="B65" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L65" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N65" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P65" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17">
+      <c r="A66" s="1">
+        <v>1</v>
+      </c>
+      <c r="B66" s="1">
+        <v>0.0003</v>
+      </c>
+      <c r="C66" s="1">
+        <v>1</v>
+      </c>
+      <c r="D66" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E66" s="1">
+        <v>16</v>
+      </c>
+      <c r="F66" s="1">
+        <v>32</v>
+      </c>
+      <c r="G66" s="2">
+        <v>0.958</v>
+      </c>
+      <c r="H66" s="1">
+        <v>0.0507</v>
+      </c>
+      <c r="I66" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J66" s="2">
+        <v>0.00141</v>
+      </c>
+      <c r="K66" s="3">
+        <f t="shared" ref="K66:K71" si="24">J66*1000*250*200</f>
+        <v>70500</v>
+      </c>
+      <c r="L66" s="2">
+        <v>0.0002</v>
+      </c>
+      <c r="M66" s="3">
+        <f t="shared" ref="M66:M71" si="25">L66*1000*250*200</f>
+        <v>10000</v>
+      </c>
+      <c r="N66" s="2">
+        <v>0.111</v>
+      </c>
+      <c r="O66" s="3">
+        <f t="shared" ref="O66:O71" si="26">N66*1000*250*200</f>
+        <v>5550000</v>
+      </c>
+      <c r="P66" s="2">
+        <v>0.887</v>
+      </c>
+      <c r="Q66" s="3">
+        <f t="shared" si="22"/>
+        <v>44350000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17">
+      <c r="A67" s="1">
+        <v>2</v>
+      </c>
+      <c r="B67" s="1">
+        <v>0.0003</v>
+      </c>
+      <c r="C67" s="1">
+        <v>1</v>
+      </c>
+      <c r="D67" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E67" s="1">
+        <v>16</v>
+      </c>
+      <c r="F67" s="1">
+        <v>32</v>
+      </c>
+      <c r="G67" s="2">
+        <v>0.954</v>
+      </c>
+      <c r="H67" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="I67" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J67" s="2">
+        <v>0.00149</v>
+      </c>
+      <c r="K67" s="3">
+        <f t="shared" si="24"/>
+        <v>74500</v>
+      </c>
+      <c r="L67" s="2">
+        <v>0.000122</v>
+      </c>
+      <c r="M67" s="3">
+        <f t="shared" si="25"/>
+        <v>6100</v>
+      </c>
+      <c r="N67" s="2">
+        <v>0.151</v>
+      </c>
+      <c r="O67" s="3">
+        <f t="shared" si="26"/>
+        <v>7550000</v>
+      </c>
+      <c r="P67" s="2">
+        <v>0.847</v>
+      </c>
+      <c r="Q67" s="3">
+        <f t="shared" si="22"/>
+        <v>42350000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17">
+      <c r="A68" s="1">
+        <v>3</v>
+      </c>
+      <c r="B68" s="1">
+        <v>0.0003</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1</v>
+      </c>
+      <c r="D68" s="1">
+        <v>100000</v>
+      </c>
+      <c r="E68" s="1">
+        <v>16</v>
+      </c>
+      <c r="F68" s="1">
+        <v>32</v>
+      </c>
+      <c r="G68" s="2">
+        <v>0.962</v>
+      </c>
+      <c r="H68" s="1">
+        <v>0.0588</v>
+      </c>
+      <c r="I68" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J68" s="2">
+        <v>0.00114</v>
+      </c>
+      <c r="K68" s="3">
+        <f t="shared" si="24"/>
+        <v>57000</v>
+      </c>
+      <c r="L68" s="2">
+        <v>0.000555</v>
+      </c>
+      <c r="M68" s="3">
+        <f t="shared" si="25"/>
+        <v>27750</v>
+      </c>
+      <c r="N68" s="2">
+        <v>0.0212</v>
+      </c>
+      <c r="O68" s="3">
+        <f t="shared" si="26"/>
+        <v>1060000</v>
+      </c>
+      <c r="P68" s="2">
+        <v>0.977</v>
+      </c>
+      <c r="Q68" s="3">
+        <f t="shared" si="22"/>
+        <v>48850000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17">
+      <c r="A69" s="1">
+        <v>4</v>
+      </c>
+      <c r="B69" s="1">
+        <v>0.0003</v>
+      </c>
+      <c r="C69" s="1">
+        <v>1</v>
+      </c>
+      <c r="D69" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E69" s="1">
+        <v>16</v>
+      </c>
+      <c r="F69" s="1">
+        <v>32</v>
+      </c>
+      <c r="G69" s="2">
+        <v>0.958</v>
+      </c>
+      <c r="H69" s="1">
+        <v>0.0594</v>
+      </c>
+      <c r="I69" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J69" s="2">
+        <v>0.000648</v>
+      </c>
+      <c r="K69" s="3">
+        <f t="shared" si="24"/>
+        <v>32400</v>
+      </c>
+      <c r="L69" s="2">
+        <v>0.000959</v>
+      </c>
+      <c r="M69" s="3">
+        <f t="shared" si="25"/>
+        <v>47950</v>
+      </c>
+      <c r="N69" s="2">
+        <v>0.00858</v>
+      </c>
+      <c r="O69" s="3">
+        <f t="shared" si="26"/>
+        <v>429000</v>
+      </c>
+      <c r="P69" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="Q69" s="3">
+        <f t="shared" si="22"/>
+        <v>49500000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17">
+      <c r="A70" s="1">
+        <v>5</v>
+      </c>
+      <c r="B70" s="1">
+        <v>0.0003</v>
+      </c>
+      <c r="C70" s="1">
+        <v>1</v>
+      </c>
+      <c r="D70" s="1">
+        <v>50000000</v>
+      </c>
+      <c r="E70" s="1">
+        <v>16</v>
+      </c>
+      <c r="F70" s="1">
+        <v>32</v>
+      </c>
+      <c r="G70" s="2">
+        <v>0.952</v>
+      </c>
+      <c r="H70" s="1">
+        <v>0.0537</v>
+      </c>
+      <c r="I70" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J70" s="2">
+        <v>0.00117</v>
+      </c>
+      <c r="K70" s="3">
+        <f t="shared" si="24"/>
+        <v>58500</v>
+      </c>
+      <c r="L70" s="2">
+        <v>0.000439</v>
+      </c>
+      <c r="M70" s="3">
+        <f t="shared" si="25"/>
+        <v>21950</v>
+      </c>
+      <c r="N70" s="2">
+        <v>0.0356</v>
+      </c>
+      <c r="O70" s="3">
+        <f t="shared" si="26"/>
+        <v>1780000</v>
+      </c>
+      <c r="P70" s="2">
+        <v>0.963</v>
+      </c>
+      <c r="Q70" s="3">
+        <f t="shared" si="22"/>
+        <v>48150000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17">
+      <c r="A71" s="1">
+        <v>6</v>
+      </c>
+      <c r="B71" s="1">
+        <v>0.0003</v>
+      </c>
+      <c r="C71" s="1">
+        <v>4</v>
+      </c>
+      <c r="D71" s="1">
+        <v>2000000</v>
+      </c>
+      <c r="E71" s="1">
+        <v>16</v>
+      </c>
+      <c r="F71" s="1">
+        <v>32</v>
+      </c>
+      <c r="G71" s="2">
+        <v>0.962</v>
+      </c>
+      <c r="H71" s="1">
+        <v>0.0571</v>
+      </c>
+      <c r="I71" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J71" s="2">
+        <v>0.00155</v>
+      </c>
+      <c r="K71" s="3">
+        <f t="shared" si="24"/>
+        <v>77500</v>
+      </c>
+      <c r="L71" s="2">
+        <v>5.23e-5</v>
+      </c>
+      <c r="M71" s="3">
+        <f t="shared" si="25"/>
+        <v>2615</v>
+      </c>
+      <c r="N71" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="O71" s="3">
+        <f t="shared" si="26"/>
+        <v>9000000</v>
+      </c>
+      <c r="P71" s="2">
+        <v>0.818</v>
+      </c>
+      <c r="Q71" s="3">
+        <f t="shared" si="22"/>
+        <v>40900000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
-      <c r="G66" s="8"/>
-      <c r="H66" s="4"/>
-    </row>
-    <row r="67" spans="2:8">
-      <c r="B67" s="1" t="s">
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="4"/>
+    </row>
+    <row r="79" spans="2:8">
+      <c r="B79" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="G79" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H67" s="1" t="s">
+      <c r="H79" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="2:8">
-      <c r="B68" s="1">
+    <row r="80" spans="2:8">
+      <c r="B80" s="1">
         <v>4</v>
       </c>
-      <c r="G68" s="2" t="s">
+      <c r="G80" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H68" s="1" t="s">
+      <c r="H80" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="69" spans="2:8">
-      <c r="B69" s="1">
+    <row r="81" spans="2:8">
+      <c r="B81" s="1">
         <v>6</v>
       </c>
-      <c r="G69" s="2" t="s">
+      <c r="G81" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="H69" s="1" t="s">
+      <c r="H81" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="70" spans="2:8">
-      <c r="B70" s="1">
+    <row r="82" spans="2:8">
+      <c r="B82" s="1">
         <v>8</v>
       </c>
-      <c r="G70" s="2" t="s">
+      <c r="G82" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H70" s="1" t="s">
+      <c r="H82" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="71" spans="2:8">
-      <c r="B71" s="1">
+    <row r="83" spans="2:8">
+      <c r="B83" s="1">
         <v>10</v>
       </c>
-      <c r="G71" s="2" t="s">
+      <c r="G83" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H71" s="1" t="s">
+      <c r="H83" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="72" spans="2:8">
-      <c r="B72" s="1">
+    <row r="84" spans="2:8">
+      <c r="B84" s="1">
         <v>12</v>
       </c>
-      <c r="G72" s="2" t="s">
+      <c r="G84" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="H72" s="1" t="s">
+      <c r="H84" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="73" spans="2:8">
-      <c r="B73" s="1">
+    <row r="85" spans="2:8">
+      <c r="B85" s="1">
         <v>14</v>
       </c>
-      <c r="G73" s="2" t="s">
+      <c r="G85" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="H73" s="1" t="s">
+      <c r="H85" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="74" spans="2:8">
-      <c r="B74" s="1">
+    <row r="86" spans="2:8">
+      <c r="B86" s="1">
         <v>16</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="G86" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="H74" s="1" t="s">
+      <c r="H86" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="75" spans="2:8">
-      <c r="B75" s="1">
+    <row r="87" spans="2:8">
+      <c r="B87" s="1">
         <v>18</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="G87" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="H75" s="1" t="s">
+      <c r="H87" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="76" spans="2:8">
-      <c r="B76" s="1">
+    <row r="88" spans="2:8">
+      <c r="B88" s="1">
         <v>20</v>
       </c>
-      <c r="G76" s="2" t="s">
+      <c r="G88" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="H76" s="1" t="s">
+      <c r="H88" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
-      <c r="A80" s="1" t="s">
+    <row r="92" spans="1:1">
+      <c r="A92" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="81" spans="2:3">
-      <c r="B81" s="1" t="s">
+    <row r="93" spans="2:3">
+      <c r="B93" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C93" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="1" t="s">
+    <row r="94" spans="1:3">
+      <c r="A94" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B94" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C94" s="1">
         <v>0.0049</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="1" t="s">
+    <row r="95" spans="1:3">
+      <c r="A95" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B95" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C83" s="1">
+      <c r="C95" s="1">
         <v>0.0001</v>
       </c>
     </row>
@@ -3949,7 +4329,7 @@
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A53:F53"/>
     <mergeCell ref="A60:F60"/>
-    <mergeCell ref="A66:H66"/>
+    <mergeCell ref="A78:H78"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Added dots for chosing of rev_log_bias to the table
</commit_message>
<xml_diff>
--- a/LSTM_all_experiments.xlsx
+++ b/LSTM_all_experiments.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="139">
   <si>
     <t>RNN</t>
   </si>
@@ -335,6 +335,15 @@
     <t>High resolution</t>
   </si>
   <si>
+    <t>RTL</t>
+  </si>
+  <si>
+    <t>Threshold = 3.5</t>
+  </si>
+  <si>
+    <t>Improvement of mean</t>
+  </si>
+  <si>
     <t>Boosting</t>
   </si>
   <si>
@@ -410,13 +419,19 @@
     <t>0.0016</t>
   </si>
   <si>
-    <t>Reversed softmax</t>
+    <t>M_heavy = 3,5</t>
   </si>
   <si>
     <t>bias</t>
   </si>
   <si>
     <t>0.0003</t>
+  </si>
+  <si>
+    <t>M_heavy = 5</t>
+  </si>
+  <si>
+    <t>Experiment</t>
   </si>
 </sst>
 </file>
@@ -425,9 +440,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -444,73 +459,22 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -532,7 +496,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -540,7 +511,76 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -553,14 +593,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -568,33 +600,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -609,7 +624,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -621,25 +660,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,7 +678,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -663,19 +708,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -687,55 +720,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -753,7 +744,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -765,13 +786,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -783,13 +798,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -821,6 +836,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -845,19 +884,27 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -878,43 +925,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -923,138 +938,138 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1408,10 +1423,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:Q111"/>
+  <dimension ref="A3:Q156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="H108" sqref="H105:H108"/>
+    <sheetView tabSelected="1" topLeftCell="B115" workbookViewId="0">
+      <selection activeCell="E138" sqref="E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1427,7 +1442,7 @@
     <col min="9" max="9" width="9" style="1" customWidth="1"/>
     <col min="10" max="10" width="12.25" style="2" customWidth="1"/>
     <col min="11" max="11" width="10.75" style="3" customWidth="1"/>
-    <col min="12" max="12" width="9" style="2" customWidth="1"/>
+    <col min="12" max="12" width="10.125" style="2" customWidth="1"/>
     <col min="13" max="13" width="9" style="3" customWidth="1"/>
     <col min="14" max="14" width="9" style="2" customWidth="1"/>
     <col min="15" max="15" width="9.375" style="3"/>
@@ -4186,671 +4201,514 @@
         <v>40900000</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
-      <c r="A78" s="4" t="s">
+    <row r="73" spans="1:2">
+      <c r="A73" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="4"/>
-      <c r="C78" s="4"/>
-      <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4"/>
-      <c r="G78" s="8"/>
-      <c r="H78" s="4"/>
-    </row>
-    <row r="79" spans="2:8">
-      <c r="B79" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G79" s="2" t="s">
+    </row>
+    <row r="74" spans="2:16">
+      <c r="B74" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G74" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H79" s="1" t="s">
+      <c r="H74" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="80" spans="2:8">
-      <c r="B80" s="1">
+      <c r="I74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N74" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P74" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16">
+      <c r="A75" s="1">
+        <v>1</v>
+      </c>
+      <c r="B75" s="1">
+        <v>0.0003</v>
+      </c>
+      <c r="C75" s="1">
+        <v>3</v>
+      </c>
+      <c r="D75" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E75" s="1">
+        <v>32</v>
+      </c>
+      <c r="F75" s="1">
+        <v>48</v>
+      </c>
+      <c r="G75" s="2">
+        <v>0.9305</v>
+      </c>
+      <c r="H75" s="1">
+        <v>0.063</v>
+      </c>
+      <c r="I75" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J75" s="2">
+        <v>0.0015</v>
+      </c>
+      <c r="L75" s="2">
+        <v>0.000111</v>
+      </c>
+      <c r="N75" s="2">
+        <v>0.314</v>
+      </c>
+      <c r="P75" s="2">
+        <v>0.685</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16">
+      <c r="A76" s="1">
+        <v>2</v>
+      </c>
+      <c r="B76" s="1">
+        <v>0.0003</v>
+      </c>
+      <c r="C76" s="1">
+        <v>3</v>
+      </c>
+      <c r="D76" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E76" s="1">
+        <v>64</v>
+      </c>
+      <c r="F76" s="1">
+        <v>64</v>
+      </c>
+      <c r="G76" s="2">
+        <v>0.923</v>
+      </c>
+      <c r="H76" s="1">
+        <v>0.0709</v>
+      </c>
+      <c r="I76" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J76" s="2">
+        <v>0.0015</v>
+      </c>
+      <c r="L76" s="2">
+        <v>0.000106</v>
+      </c>
+      <c r="N76" s="2">
+        <v>0.288</v>
+      </c>
+      <c r="P76" s="2">
+        <v>0.711</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16">
+      <c r="A77" s="1">
+        <v>3</v>
+      </c>
+      <c r="B77" s="1">
+        <v>0.0003</v>
+      </c>
+      <c r="C77" s="1">
+        <v>3</v>
+      </c>
+      <c r="D77" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E77" s="1">
+        <v>100</v>
+      </c>
+      <c r="F77" s="1">
+        <v>100</v>
+      </c>
+      <c r="G77" s="2">
+        <v>0.941</v>
+      </c>
+      <c r="H77" s="1">
+        <v>0.0658</v>
+      </c>
+      <c r="I77" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J77" s="2">
+        <v>0.00155</v>
+      </c>
+      <c r="L77" s="2">
+        <v>5.78e-5</v>
+      </c>
+      <c r="N77" s="2">
+        <v>0.406</v>
+      </c>
+      <c r="P77" s="2">
+        <v>0.593</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16">
+      <c r="A78" s="1">
         <v>4</v>
       </c>
-      <c r="G80" s="2" t="s">
+      <c r="B78" s="1">
+        <v>0.0003</v>
+      </c>
+      <c r="C78" s="1">
+        <v>3</v>
+      </c>
+      <c r="D78" s="1">
+        <v>100000</v>
+      </c>
+      <c r="E78" s="1">
+        <v>64</v>
+      </c>
+      <c r="F78" s="1">
+        <v>64</v>
+      </c>
+      <c r="G78" s="2">
+        <v>0.935</v>
+      </c>
+      <c r="H78" s="1">
+        <v>0.0647</v>
+      </c>
+      <c r="I78" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J78" s="2">
+        <v>0.00155</v>
+      </c>
+      <c r="L78" s="2">
+        <v>6.14e-5</v>
+      </c>
+      <c r="N78" s="2">
+        <v>0.436</v>
+      </c>
+      <c r="P78" s="2">
+        <v>0.562</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="H80" s="1" t="s">
+      <c r="B80" s="7"/>
+    </row>
+    <row r="81" spans="2:16">
+      <c r="B81" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J81" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L81" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N81" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P81" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16">
+      <c r="A82" s="1">
+        <v>1</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C82" s="1">
+        <v>1</v>
+      </c>
+      <c r="D82" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E82" s="1">
+        <v>16</v>
+      </c>
+      <c r="F82" s="1">
+        <v>32</v>
+      </c>
+      <c r="G82" s="2">
+        <v>0.956</v>
+      </c>
+      <c r="H82" s="1">
+        <v>0.075</v>
+      </c>
+      <c r="I82" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J82" s="2">
+        <v>0.00156</v>
+      </c>
+      <c r="L82" s="2">
+        <v>4.54e-5</v>
+      </c>
+      <c r="N82" s="2">
+        <v>0.252</v>
+      </c>
+      <c r="P82" s="2">
+        <v>0.765</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="81" spans="2:8">
-      <c r="B81" s="1">
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="8"/>
+      <c r="H86" s="4"/>
+    </row>
+    <row r="87" spans="2:8">
+      <c r="B87" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H87" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H81" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="82" spans="2:8">
-      <c r="B82" s="1">
-        <v>8</v>
-      </c>
-      <c r="G82" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H82" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="83" spans="2:8">
-      <c r="B83" s="1">
-        <v>10</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H83" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="84" spans="2:8">
-      <c r="B84" s="1">
-        <v>12</v>
-      </c>
-      <c r="G84" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="85" spans="2:8">
-      <c r="B85" s="1">
-        <v>14</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="86" spans="2:8">
-      <c r="B86" s="1">
-        <v>16</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="H86" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="87" spans="2:8">
-      <c r="B87" s="1">
-        <v>18</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H87" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="88" spans="2:8">
       <c r="B88" s="1">
+        <v>4</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8">
+      <c r="B89" s="1">
+        <v>6</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8">
+      <c r="B90" s="1">
+        <v>8</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8">
+      <c r="B91" s="1">
+        <v>10</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8">
+      <c r="B92" s="1">
+        <v>12</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8">
+      <c r="B93" s="1">
+        <v>14</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8">
+      <c r="B94" s="1">
+        <v>16</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8">
+      <c r="B95" s="1">
+        <v>18</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8">
+      <c r="B96" s="1">
         <v>20</v>
       </c>
-      <c r="G88" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="H88" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1">
-      <c r="A92" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="93" spans="2:3">
-      <c r="B93" s="1" t="s">
+      <c r="G96" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="H96" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
-      <c r="A94" s="1" t="s">
+    <row r="100" spans="1:1">
+      <c r="A100" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B94" s="1" t="s">
+    </row>
+    <row r="101" spans="2:3">
+      <c r="B101" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C101" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C102" s="1">
         <v>0.0049</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
-      <c r="A95" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C95" s="1">
-        <v>0.0001</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5">
-      <c r="A97" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B97" s="7"/>
-      <c r="C97" s="7"/>
-      <c r="D97" s="7"/>
-      <c r="E97" s="7"/>
-    </row>
-    <row r="98" spans="1:16">
-      <c r="A98" s="1" t="s">
+    <row r="103" spans="1:3">
+      <c r="A103" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H98" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I98" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J98" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L98" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N98" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P98" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="99" spans="1:16">
-      <c r="A99" s="1">
-        <v>0</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C99" s="1">
-        <v>1</v>
-      </c>
-      <c r="D99" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E99" s="1">
-        <v>16</v>
-      </c>
-      <c r="F99" s="1">
-        <v>32</v>
-      </c>
-      <c r="G99" s="2">
-        <v>0.974</v>
-      </c>
-      <c r="H99" s="1">
-        <v>0.077</v>
-      </c>
-      <c r="I99" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="J99" s="2">
-        <v>0.0012</v>
-      </c>
-      <c r="L99" s="2">
-        <v>0.000403</v>
-      </c>
-      <c r="N99" s="2">
-        <v>0.0356</v>
-      </c>
-      <c r="P99" s="2">
-        <v>0.963</v>
-      </c>
-    </row>
-    <row r="100" spans="1:16">
-      <c r="A100" s="1">
-        <v>0</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C100" s="1">
-        <v>1</v>
-      </c>
-      <c r="D100" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E100" s="1">
-        <v>16</v>
-      </c>
-      <c r="F100" s="1">
-        <v>32</v>
-      </c>
-      <c r="G100" s="2">
-        <v>0.973</v>
-      </c>
-      <c r="H100" s="1">
-        <v>0.085</v>
-      </c>
-      <c r="I100" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="J100" s="2">
-        <v>0.00085</v>
-      </c>
-      <c r="L100" s="2">
-        <v>0.000759</v>
-      </c>
-      <c r="N100" s="2">
-        <v>0.0116</v>
-      </c>
-      <c r="O100" s="3"/>
-      <c r="P100" s="2">
-        <v>0.987</v>
-      </c>
-    </row>
-    <row r="101" spans="1:16">
-      <c r="A101" s="1">
-        <v>0</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C101" s="1">
-        <v>1</v>
-      </c>
-      <c r="D101" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E101" s="1">
-        <v>16</v>
-      </c>
-      <c r="F101" s="1">
-        <v>32</v>
-      </c>
-      <c r="G101" s="2">
-        <v>0.974</v>
-      </c>
-      <c r="H101" s="1">
-        <v>0.0846</v>
-      </c>
-      <c r="I101" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="J101" s="2">
-        <v>0.00108</v>
-      </c>
-      <c r="L101" s="2">
-        <v>0.000527</v>
-      </c>
-      <c r="N101" s="2">
-        <v>0.0247</v>
-      </c>
-      <c r="P101" s="2">
-        <v>0.974</v>
-      </c>
-    </row>
-    <row r="102" spans="1:16">
-      <c r="A102" s="1">
-        <v>-1</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C102" s="1">
-        <v>1</v>
-      </c>
-      <c r="D102" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E102" s="1">
-        <v>16</v>
-      </c>
-      <c r="F102" s="1">
-        <v>32</v>
-      </c>
-      <c r="G102" s="2">
-        <v>0.973</v>
-      </c>
-      <c r="H102" s="1">
-        <v>0.0828</v>
-      </c>
-      <c r="I102" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="J102" s="2">
-        <v>0.000958</v>
-      </c>
-      <c r="L102" s="2">
-        <v>0.000648</v>
-      </c>
-      <c r="N102" s="2">
-        <v>0.0202</v>
-      </c>
-      <c r="P102" s="2">
-        <v>0.978</v>
-      </c>
-    </row>
-    <row r="103" spans="1:16">
-      <c r="A103" s="1">
-        <v>-1</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>133</v>
       </c>
       <c r="C103" s="1">
-        <v>1</v>
-      </c>
-      <c r="D103" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E103" s="1">
-        <v>16</v>
-      </c>
-      <c r="F103" s="1">
-        <v>32</v>
-      </c>
-      <c r="G103" s="2">
-        <v>0.974</v>
-      </c>
-      <c r="H103" s="1">
-        <v>0.0858</v>
-      </c>
-      <c r="I103" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="J103" s="2">
-        <v>0.000999</v>
-      </c>
-      <c r="L103" s="2">
-        <v>0.000652</v>
-      </c>
-      <c r="N103" s="2">
-        <v>0.0156</v>
-      </c>
-      <c r="P103" s="2">
-        <v>0.983</v>
-      </c>
-    </row>
-    <row r="104" spans="1:16">
-      <c r="A104" s="1">
-        <v>-1</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C104" s="1">
-        <v>1</v>
-      </c>
-      <c r="D104" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E104" s="1">
-        <v>16</v>
-      </c>
-      <c r="F104" s="1">
-        <v>32</v>
-      </c>
-      <c r="G104" s="2">
-        <v>0.975</v>
-      </c>
-      <c r="H104" s="1">
-        <v>0.0814</v>
-      </c>
-      <c r="I104" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="J104" s="2">
-        <v>0.00125</v>
-      </c>
-      <c r="L104" s="2">
-        <v>0.000353</v>
-      </c>
-      <c r="N104" s="2">
-        <v>0.0383</v>
-      </c>
-      <c r="P104" s="2">
-        <v>0.96</v>
-      </c>
-    </row>
-    <row r="105" spans="1:16">
-      <c r="A105" s="1">
-        <v>1</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C105" s="1">
-        <v>1</v>
-      </c>
-      <c r="D105" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E105" s="1">
-        <v>16</v>
-      </c>
-      <c r="F105" s="1">
-        <v>32</v>
-      </c>
-      <c r="G105" s="2">
-        <v>0.975</v>
-      </c>
-      <c r="H105" s="1">
-        <v>0.0868</v>
-      </c>
-      <c r="I105" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="J105" s="2">
-        <v>0.00105</v>
-      </c>
-      <c r="L105" s="2">
-        <v>0.000555</v>
-      </c>
-      <c r="N105" s="2">
-        <v>0.0217</v>
-      </c>
-      <c r="P105" s="2">
-        <v>0.977</v>
-      </c>
-    </row>
-    <row r="106" spans="1:16">
-      <c r="A106" s="1">
-        <v>1</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C106" s="1">
-        <v>1</v>
-      </c>
-      <c r="D106" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E106" s="1">
-        <v>16</v>
-      </c>
-      <c r="F106" s="1">
-        <v>32</v>
-      </c>
-      <c r="G106" s="2">
-        <v>0.975</v>
-      </c>
-      <c r="H106" s="1">
-        <v>0.089</v>
-      </c>
-      <c r="I106" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="J106" s="2">
-        <v>0.0011</v>
-      </c>
-      <c r="L106" s="2">
-        <v>0.000504</v>
-      </c>
-      <c r="N106" s="2">
-        <v>0.0246</v>
-      </c>
-      <c r="P106" s="2">
-        <v>0.974</v>
-      </c>
-    </row>
-    <row r="107" spans="1:16">
-      <c r="A107" s="1">
-        <v>1</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C107" s="1">
-        <v>1</v>
-      </c>
-      <c r="D107" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E107" s="1">
-        <v>16</v>
-      </c>
-      <c r="F107" s="1">
-        <v>32</v>
-      </c>
-      <c r="G107" s="2">
-        <v>0.974</v>
-      </c>
-      <c r="H107" s="1">
-        <v>0.0877</v>
-      </c>
-      <c r="I107" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="J107" s="2">
-        <v>0.00104</v>
-      </c>
-      <c r="L107" s="2">
-        <v>0.000563</v>
-      </c>
-      <c r="N107" s="2">
-        <v>0.0212</v>
-      </c>
-      <c r="P107" s="2">
-        <v>0.977</v>
-      </c>
-    </row>
-    <row r="108" spans="1:16">
-      <c r="A108" s="1">
-        <v>1</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C108" s="1">
-        <v>1</v>
-      </c>
-      <c r="D108" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E108" s="1">
-        <v>16</v>
-      </c>
-      <c r="F108" s="1">
-        <v>32</v>
-      </c>
-      <c r="G108" s="2">
-        <v>0.975</v>
-      </c>
-      <c r="H108" s="1">
-        <v>0.0847</v>
-      </c>
-      <c r="I108" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="J108" s="2">
-        <v>0.00107</v>
-      </c>
-      <c r="L108" s="2">
-        <v>0.000536</v>
-      </c>
-      <c r="N108" s="2">
-        <v>0.0233</v>
-      </c>
-      <c r="P108" s="2">
-        <v>0.975</v>
-      </c>
+        <v>0.0001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B108" s="7"/>
+      <c r="C108" s="7"/>
+      <c r="D108" s="7"/>
+      <c r="E108" s="7"/>
     </row>
     <row r="109" spans="1:16">
-      <c r="A109" s="1">
-        <v>2</v>
+      <c r="A109" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C109" s="1">
-        <v>1</v>
-      </c>
-      <c r="D109" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E109" s="1">
-        <v>16</v>
-      </c>
-      <c r="F109" s="1">
-        <v>32</v>
-      </c>
-      <c r="G109" s="2">
-        <v>0.974</v>
-      </c>
-      <c r="H109" s="1">
-        <v>0.0726</v>
-      </c>
-      <c r="I109" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="J109" s="2">
-        <v>0.00102</v>
-      </c>
-      <c r="L109" s="2">
-        <v>0.000589</v>
-      </c>
-      <c r="N109" s="2">
-        <v>0.0204</v>
-      </c>
-      <c r="P109" s="2">
-        <v>0.978</v>
+        <v>84</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J109" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L109" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N109" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P109" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="110" spans="1:16">
       <c r="A110" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C110" s="1">
         <v>1</v>
@@ -4868,30 +4726,30 @@
         <v>0.974</v>
       </c>
       <c r="H110" s="1">
-        <v>0.0835</v>
+        <v>0.077</v>
       </c>
       <c r="I110" s="1">
         <v>0.6</v>
       </c>
       <c r="J110" s="2">
-        <v>0.00104</v>
+        <v>0.0012</v>
       </c>
       <c r="L110" s="2">
-        <v>0.000552</v>
+        <v>0.000403</v>
       </c>
       <c r="N110" s="2">
-        <v>0.0259</v>
+        <v>0.0356</v>
       </c>
       <c r="P110" s="2">
-        <v>0.975</v>
+        <v>0.963</v>
       </c>
     </row>
     <row r="111" spans="1:16">
       <c r="A111" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C111" s="1">
         <v>1</v>
@@ -4909,26 +4767,1273 @@
         <v>0.973</v>
       </c>
       <c r="H111" s="1">
-        <v>0.0804</v>
+        <v>0.085</v>
       </c>
       <c r="I111" s="1">
         <v>0.6</v>
       </c>
       <c r="J111" s="2">
+        <v>0.00085</v>
+      </c>
+      <c r="L111" s="2">
+        <v>0.000759</v>
+      </c>
+      <c r="N111" s="2">
+        <v>0.0116</v>
+      </c>
+      <c r="P111" s="2">
+        <v>0.987</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16">
+      <c r="A112" s="1">
+        <v>0</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C112" s="1">
+        <v>1</v>
+      </c>
+      <c r="D112" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E112" s="1">
+        <v>16</v>
+      </c>
+      <c r="F112" s="1">
+        <v>32</v>
+      </c>
+      <c r="G112" s="2">
+        <v>0.974</v>
+      </c>
+      <c r="H112" s="1">
+        <v>0.0846</v>
+      </c>
+      <c r="I112" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J112" s="2">
+        <v>0.00108</v>
+      </c>
+      <c r="L112" s="2">
+        <v>0.000527</v>
+      </c>
+      <c r="N112" s="2">
+        <v>0.0247</v>
+      </c>
+      <c r="P112" s="2">
+        <v>0.974</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16">
+      <c r="A113" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C113" s="1">
+        <v>1</v>
+      </c>
+      <c r="D113" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E113" s="1">
+        <v>16</v>
+      </c>
+      <c r="F113" s="1">
+        <v>32</v>
+      </c>
+      <c r="G113" s="2">
+        <v>0.973</v>
+      </c>
+      <c r="H113" s="1">
+        <v>0.0828</v>
+      </c>
+      <c r="I113" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J113" s="2">
+        <v>0.000958</v>
+      </c>
+      <c r="L113" s="2">
+        <v>0.000648</v>
+      </c>
+      <c r="N113" s="2">
+        <v>0.0202</v>
+      </c>
+      <c r="P113" s="2">
+        <v>0.978</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16">
+      <c r="A114" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C114" s="1">
+        <v>1</v>
+      </c>
+      <c r="D114" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E114" s="1">
+        <v>16</v>
+      </c>
+      <c r="F114" s="1">
+        <v>32</v>
+      </c>
+      <c r="G114" s="2">
+        <v>0.974</v>
+      </c>
+      <c r="H114" s="1">
+        <v>0.0858</v>
+      </c>
+      <c r="I114" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J114" s="2">
+        <v>0.000999</v>
+      </c>
+      <c r="L114" s="2">
+        <v>0.000652</v>
+      </c>
+      <c r="N114" s="2">
+        <v>0.0156</v>
+      </c>
+      <c r="P114" s="2">
+        <v>0.983</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16">
+      <c r="A115" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C115" s="1">
+        <v>1</v>
+      </c>
+      <c r="D115" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E115" s="1">
+        <v>16</v>
+      </c>
+      <c r="F115" s="1">
+        <v>32</v>
+      </c>
+      <c r="G115" s="2">
+        <v>0.975</v>
+      </c>
+      <c r="H115" s="1">
+        <v>0.0814</v>
+      </c>
+      <c r="I115" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J115" s="2">
+        <v>0.00125</v>
+      </c>
+      <c r="L115" s="2">
+        <v>0.000353</v>
+      </c>
+      <c r="N115" s="2">
+        <v>0.0383</v>
+      </c>
+      <c r="P115" s="2">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16">
+      <c r="A116" s="1">
+        <v>1</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C116" s="1">
+        <v>1</v>
+      </c>
+      <c r="D116" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E116" s="1">
+        <v>16</v>
+      </c>
+      <c r="F116" s="1">
+        <v>32</v>
+      </c>
+      <c r="G116" s="2">
+        <v>0.975</v>
+      </c>
+      <c r="H116" s="1">
+        <v>0.0868</v>
+      </c>
+      <c r="I116" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J116" s="2">
+        <v>0.00105</v>
+      </c>
+      <c r="L116" s="2">
+        <v>0.000555</v>
+      </c>
+      <c r="N116" s="2">
+        <v>0.0217</v>
+      </c>
+      <c r="P116" s="2">
+        <v>0.977</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16">
+      <c r="A117" s="1">
+        <v>1</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C117" s="1">
+        <v>1</v>
+      </c>
+      <c r="D117" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E117" s="1">
+        <v>16</v>
+      </c>
+      <c r="F117" s="1">
+        <v>32</v>
+      </c>
+      <c r="G117" s="2">
+        <v>0.975</v>
+      </c>
+      <c r="H117" s="1">
+        <v>0.089</v>
+      </c>
+      <c r="I117" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J117" s="2">
+        <v>0.0011</v>
+      </c>
+      <c r="L117" s="2">
+        <v>0.000504</v>
+      </c>
+      <c r="N117" s="2">
+        <v>0.0246</v>
+      </c>
+      <c r="P117" s="2">
+        <v>0.974</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16">
+      <c r="A118" s="1">
+        <v>1</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C118" s="1">
+        <v>1</v>
+      </c>
+      <c r="D118" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E118" s="1">
+        <v>16</v>
+      </c>
+      <c r="F118" s="1">
+        <v>32</v>
+      </c>
+      <c r="G118" s="2">
+        <v>0.974</v>
+      </c>
+      <c r="H118" s="1">
+        <v>0.0877</v>
+      </c>
+      <c r="I118" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J118" s="2">
+        <v>0.00104</v>
+      </c>
+      <c r="L118" s="2">
+        <v>0.000563</v>
+      </c>
+      <c r="N118" s="2">
+        <v>0.0212</v>
+      </c>
+      <c r="P118" s="2">
+        <v>0.977</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16">
+      <c r="A119" s="1">
+        <v>1</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C119" s="1">
+        <v>1</v>
+      </c>
+      <c r="D119" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E119" s="1">
+        <v>16</v>
+      </c>
+      <c r="F119" s="1">
+        <v>32</v>
+      </c>
+      <c r="G119" s="2">
+        <v>0.975</v>
+      </c>
+      <c r="H119" s="1">
+        <v>0.0847</v>
+      </c>
+      <c r="I119" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J119" s="2">
+        <v>0.00107</v>
+      </c>
+      <c r="L119" s="2">
+        <v>0.000536</v>
+      </c>
+      <c r="N119" s="2">
+        <v>0.0233</v>
+      </c>
+      <c r="P119" s="2">
+        <v>0.975</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16">
+      <c r="A120" s="1">
+        <v>2</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C120" s="1">
+        <v>1</v>
+      </c>
+      <c r="D120" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E120" s="1">
+        <v>16</v>
+      </c>
+      <c r="F120" s="1">
+        <v>32</v>
+      </c>
+      <c r="G120" s="2">
+        <v>0.974</v>
+      </c>
+      <c r="H120" s="1">
+        <v>0.0726</v>
+      </c>
+      <c r="I120" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J120" s="2">
+        <v>0.00102</v>
+      </c>
+      <c r="L120" s="2">
+        <v>0.000589</v>
+      </c>
+      <c r="N120" s="2">
+        <v>0.0204</v>
+      </c>
+      <c r="P120" s="2">
+        <v>0.978</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16">
+      <c r="A121" s="1">
+        <v>2</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C121" s="1">
+        <v>1</v>
+      </c>
+      <c r="D121" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E121" s="1">
+        <v>16</v>
+      </c>
+      <c r="F121" s="1">
+        <v>32</v>
+      </c>
+      <c r="G121" s="2">
+        <v>0.974</v>
+      </c>
+      <c r="H121" s="1">
+        <v>0.0835</v>
+      </c>
+      <c r="I121" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J121" s="2">
+        <v>0.00104</v>
+      </c>
+      <c r="L121" s="2">
+        <v>0.000552</v>
+      </c>
+      <c r="N121" s="2">
+        <v>0.0259</v>
+      </c>
+      <c r="P121" s="2">
+        <v>0.975</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16">
+      <c r="A122" s="1">
+        <v>2</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C122" s="1">
+        <v>1</v>
+      </c>
+      <c r="D122" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E122" s="1">
+        <v>16</v>
+      </c>
+      <c r="F122" s="1">
+        <v>32</v>
+      </c>
+      <c r="G122" s="2">
+        <v>0.973</v>
+      </c>
+      <c r="H122" s="1">
+        <v>0.0804</v>
+      </c>
+      <c r="I122" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J122" s="2">
         <v>0.000763</v>
       </c>
-      <c r="L111" s="2">
+      <c r="L122" s="2">
         <v>0.000821</v>
       </c>
-      <c r="N111" s="2">
+      <c r="N122" s="2">
         <v>0.0108</v>
       </c>
-      <c r="P111" s="2">
+      <c r="P122" s="2">
         <v>0.988</v>
       </c>
     </row>
+    <row r="126" spans="1:5">
+      <c r="A126" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B126" s="7"/>
+      <c r="C126" s="7"/>
+      <c r="D126" s="7"/>
+      <c r="E126" s="7"/>
+    </row>
+    <row r="127" spans="1:16">
+      <c r="A127" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G127" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I127" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J127" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L127" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N127" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P127" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16">
+      <c r="A128" s="1">
+        <v>0</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C128" s="1">
+        <v>1</v>
+      </c>
+      <c r="D128" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E128" s="1">
+        <v>16</v>
+      </c>
+      <c r="F128" s="1">
+        <v>32</v>
+      </c>
+      <c r="G128" s="2">
+        <v>0.9925</v>
+      </c>
+      <c r="H128" s="1">
+        <v>0.00541</v>
+      </c>
+      <c r="I128" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J128" s="2">
+        <v>1.76e-5</v>
+      </c>
+      <c r="L128" s="2">
+        <v>4.77e-5</v>
+      </c>
+      <c r="N128" s="2">
+        <v>0.0027</v>
+      </c>
+      <c r="P128" s="2">
+        <v>0.9972</v>
+      </c>
+    </row>
+    <row r="129" spans="1:16">
+      <c r="A129" s="1">
+        <v>0</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C129" s="1">
+        <v>1</v>
+      </c>
+      <c r="D129" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E129" s="1">
+        <v>16</v>
+      </c>
+      <c r="F129" s="1">
+        <v>32</v>
+      </c>
+      <c r="G129" s="2">
+        <v>0.9926</v>
+      </c>
+      <c r="H129" s="1">
+        <v>0.00614</v>
+      </c>
+      <c r="I129" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J129" s="2">
+        <v>2.54e-5</v>
+      </c>
+      <c r="L129" s="2">
+        <v>3.99e-5</v>
+      </c>
+      <c r="N129" s="2">
+        <v>0.00388</v>
+      </c>
+      <c r="P129" s="2">
+        <v>0.9961</v>
+      </c>
+    </row>
+    <row r="130" spans="1:16">
+      <c r="A130" s="1">
+        <v>0</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C130" s="1">
+        <v>1</v>
+      </c>
+      <c r="D130" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E130" s="1">
+        <v>16</v>
+      </c>
+      <c r="F130" s="1">
+        <v>32</v>
+      </c>
+      <c r="G130" s="2">
+        <v>0.993</v>
+      </c>
+      <c r="H130" s="1">
+        <v>0.00603</v>
+      </c>
+      <c r="I130" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J130" s="2">
+        <v>2.31e-5</v>
+      </c>
+      <c r="L130" s="2">
+        <v>4.22e-5</v>
+      </c>
+      <c r="N130" s="2">
+        <v>0.00338</v>
+      </c>
+      <c r="P130" s="2">
+        <v>0.9966</v>
+      </c>
+    </row>
+    <row r="131" spans="1:16">
+      <c r="A131" s="1">
+        <v>1</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C131" s="1">
+        <v>1</v>
+      </c>
+      <c r="D131" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E131" s="1">
+        <v>16</v>
+      </c>
+      <c r="F131" s="1">
+        <v>32</v>
+      </c>
+      <c r="G131" s="2">
+        <v>0.9929</v>
+      </c>
+      <c r="H131" s="1">
+        <v>0.00579</v>
+      </c>
+      <c r="I131" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J131" s="2">
+        <v>2.26e-5</v>
+      </c>
+      <c r="L131" s="2">
+        <v>4.27e-5</v>
+      </c>
+      <c r="N131" s="2">
+        <v>0.00367</v>
+      </c>
+      <c r="P131" s="2">
+        <v>0.9963</v>
+      </c>
+    </row>
+    <row r="132" spans="1:16">
+      <c r="A132" s="1">
+        <v>1</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C132" s="1">
+        <v>1</v>
+      </c>
+      <c r="D132" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E132" s="1">
+        <v>16</v>
+      </c>
+      <c r="F132" s="1">
+        <v>32</v>
+      </c>
+      <c r="G132" s="2">
+        <v>0.9926</v>
+      </c>
+      <c r="H132" s="1">
+        <v>0.00548</v>
+      </c>
+      <c r="I132" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J132" s="2">
+        <v>2.63e-5</v>
+      </c>
+      <c r="L132" s="2">
+        <v>3.9e-5</v>
+      </c>
+      <c r="N132" s="2">
+        <v>0.00435</v>
+      </c>
+      <c r="P132" s="2">
+        <v>0.9956</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16">
+      <c r="A133" s="1">
+        <v>1</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C133" s="1">
+        <v>1</v>
+      </c>
+      <c r="D133" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E133" s="1">
+        <v>16</v>
+      </c>
+      <c r="F133" s="1">
+        <v>32</v>
+      </c>
+      <c r="G133" s="2">
+        <v>0.9924</v>
+      </c>
+      <c r="H133" s="1">
+        <v>0.0057</v>
+      </c>
+      <c r="I133" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J133" s="2">
+        <v>1.81e-5</v>
+      </c>
+      <c r="L133" s="2">
+        <v>4.73e-5</v>
+      </c>
+      <c r="N133" s="2">
+        <v>0.003</v>
+      </c>
+      <c r="P133" s="2">
+        <v>0.9969</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16">
+      <c r="A134" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C134" s="1">
+        <v>1</v>
+      </c>
+      <c r="D134" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E134" s="1">
+        <v>16</v>
+      </c>
+      <c r="F134" s="1">
+        <v>32</v>
+      </c>
+      <c r="G134" s="2">
+        <v>0.9928</v>
+      </c>
+      <c r="H134" s="1">
+        <v>0.006</v>
+      </c>
+      <c r="I134" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J134" s="2">
+        <v>2.05e-5</v>
+      </c>
+      <c r="L134" s="2">
+        <v>4.48e-5</v>
+      </c>
+      <c r="N134" s="2">
+        <v>0.00328</v>
+      </c>
+      <c r="P134" s="2">
+        <v>0.9967</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16">
+      <c r="A135" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C135" s="1">
+        <v>1</v>
+      </c>
+      <c r="D135" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E135" s="1">
+        <v>16</v>
+      </c>
+      <c r="F135" s="1">
+        <v>32</v>
+      </c>
+      <c r="G135" s="2">
+        <v>0.9931</v>
+      </c>
+      <c r="H135" s="1">
+        <v>0.00653</v>
+      </c>
+      <c r="I135" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J135" s="2">
+        <v>2.6e-5</v>
+      </c>
+      <c r="L135" s="2">
+        <v>3.94e-5</v>
+      </c>
+      <c r="N135" s="2">
+        <v>0.00389</v>
+      </c>
+      <c r="P135" s="2">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16">
+      <c r="A136" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C136" s="1">
+        <v>1</v>
+      </c>
+      <c r="D136" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E136" s="1">
+        <v>16</v>
+      </c>
+      <c r="F136" s="1">
+        <v>32</v>
+      </c>
+      <c r="G136" s="2">
+        <v>0.9917</v>
+      </c>
+      <c r="H136" s="1">
+        <v>0.00525</v>
+      </c>
+      <c r="I136" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J136" s="2">
+        <v>2.6e-6</v>
+      </c>
+      <c r="L136" s="2">
+        <v>6.27e-5</v>
+      </c>
+      <c r="N136" s="2">
+        <v>0.000327</v>
+      </c>
+      <c r="P136" s="2">
+        <v>0.9996</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16">
+      <c r="A137" s="1">
+        <v>-2</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C137" s="1">
+        <v>1</v>
+      </c>
+      <c r="D137" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E137" s="1">
+        <v>16</v>
+      </c>
+      <c r="F137" s="1">
+        <v>32</v>
+      </c>
+      <c r="G137" s="2">
+        <v>0.993</v>
+      </c>
+      <c r="H137" s="1">
+        <v>0.00592</v>
+      </c>
+      <c r="I137" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J137" s="2">
+        <v>2.11e-5</v>
+      </c>
+      <c r="L137" s="2">
+        <v>4.42e-5</v>
+      </c>
+      <c r="N137" s="2">
+        <v>0.00305</v>
+      </c>
+      <c r="P137" s="2">
+        <v>0.9969</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16">
+      <c r="A138" s="1">
+        <v>-2</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C138" s="1">
+        <v>1</v>
+      </c>
+      <c r="D138" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E138" s="1">
+        <v>16</v>
+      </c>
+      <c r="F138" s="1">
+        <v>32</v>
+      </c>
+      <c r="G138" s="2">
+        <v>0.9917</v>
+      </c>
+      <c r="H138" s="1">
+        <v>0.00535</v>
+      </c>
+      <c r="I138" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J138" s="2">
+        <v>1.61e-5</v>
+      </c>
+      <c r="L138" s="2">
+        <v>4.93e-5</v>
+      </c>
+      <c r="N138" s="2">
+        <v>0.00267</v>
+      </c>
+      <c r="P138" s="2">
+        <v>0.9973</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16">
+      <c r="A139" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C139" s="1">
+        <v>1</v>
+      </c>
+      <c r="D139" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E139" s="1">
+        <v>16</v>
+      </c>
+      <c r="F139" s="1">
+        <v>32</v>
+      </c>
+      <c r="G139" s="2">
+        <v>0.9924</v>
+      </c>
+      <c r="H139" s="1">
+        <v>0.00596</v>
+      </c>
+      <c r="I139" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J139" s="2">
+        <v>2.06e-5</v>
+      </c>
+      <c r="L139" s="2">
+        <v>4.47e-5</v>
+      </c>
+      <c r="N139" s="2">
+        <v>0.00296</v>
+      </c>
+      <c r="P139" s="2">
+        <v>0.997</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B145" s="7"/>
+      <c r="C145" s="7"/>
+      <c r="D145" s="7"/>
+      <c r="E145" s="7"/>
+      <c r="F145" s="7"/>
+    </row>
+    <row r="146" spans="1:16">
+      <c r="A146" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G146" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H146" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I146" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J146" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L146" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N146" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P146" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="147" spans="1:16">
+      <c r="A147" s="1">
+        <v>0</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C147" s="1">
+        <v>1</v>
+      </c>
+      <c r="D147" s="1">
+        <v>1</v>
+      </c>
+      <c r="E147" s="1">
+        <v>16</v>
+      </c>
+      <c r="F147" s="1">
+        <v>32</v>
+      </c>
+      <c r="G147" s="2">
+        <v>0.933</v>
+      </c>
+      <c r="H147" s="1">
+        <v>0.0172</v>
+      </c>
+      <c r="I147" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J147" s="2">
+        <v>0</v>
+      </c>
+      <c r="L147" s="2">
+        <v>0.00162</v>
+      </c>
+      <c r="N147" s="2">
+        <v>0</v>
+      </c>
+      <c r="P147" s="2">
+        <v>0.9984</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" s="1">
+        <v>1</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C148" s="1">
+        <v>1</v>
+      </c>
+      <c r="D148" s="1"/>
+      <c r="E148" s="1">
+        <v>16</v>
+      </c>
+      <c r="F148" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149" s="1">
+        <v>2</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C149" s="1">
+        <v>1</v>
+      </c>
+      <c r="D149" s="1"/>
+      <c r="E149" s="1">
+        <v>16</v>
+      </c>
+      <c r="F149" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" s="1">
+        <v>3</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C150" s="1">
+        <v>1</v>
+      </c>
+      <c r="D150" s="1"/>
+      <c r="E150" s="1">
+        <v>16</v>
+      </c>
+      <c r="F150" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" s="1">
+        <v>4</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C151" s="1">
+        <v>1</v>
+      </c>
+      <c r="D151" s="1"/>
+      <c r="E151" s="1">
+        <v>16</v>
+      </c>
+      <c r="F151" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" s="1">
+        <v>5</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C152" s="1">
+        <v>1</v>
+      </c>
+      <c r="D152" s="1"/>
+      <c r="E152" s="1">
+        <v>16</v>
+      </c>
+      <c r="F152" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" s="1">
+        <v>6</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C153" s="1">
+        <v>1</v>
+      </c>
+      <c r="D153" s="1"/>
+      <c r="E153" s="1">
+        <v>16</v>
+      </c>
+      <c r="F153" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154" s="1">
+        <v>7</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C154" s="1">
+        <v>1</v>
+      </c>
+      <c r="D154" s="1"/>
+      <c r="E154" s="1">
+        <v>16</v>
+      </c>
+      <c r="F154" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
+      <c r="A155" s="1">
+        <v>8</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C155" s="1">
+        <v>1</v>
+      </c>
+      <c r="D155" s="1"/>
+      <c r="E155" s="1">
+        <v>16</v>
+      </c>
+      <c r="F155" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
+      <c r="A156" s="1">
+        <v>9</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C156" s="1">
+        <v>1</v>
+      </c>
+      <c r="D156" s="1"/>
+      <c r="E156" s="1">
+        <v>16</v>
+      </c>
+      <c r="F156" s="1">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="A38:B38"/>
@@ -4936,8 +6041,11 @@
     <mergeCell ref="A53:F53"/>
     <mergeCell ref="A60:F60"/>
     <mergeCell ref="A64:F64"/>
-    <mergeCell ref="A78:H78"/>
-    <mergeCell ref="A97:E97"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A86:H86"/>
+    <mergeCell ref="A108:E108"/>
+    <mergeCell ref="A126:E126"/>
+    <mergeCell ref="A145:F145"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>